<commit_message>
test-16 for regional saldo
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-16.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-16.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="mse (unbalanced set)" sheetId="1" r:id="rId1"/>
+    <sheet name="feature sig" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>features</t>
   </si>
@@ -88,6 +89,18 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24 reg.csv)</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
+    <t>interregional</t>
+  </si>
+  <si>
+    <t>international</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 interreg.csv)</t>
   </si>
 </sst>
 </file>
@@ -446,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:Y58"/>
+  <dimension ref="C4:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,12 +471,16 @@
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
     <col min="24" max="24" width="17.7109375" customWidth="1"/>
     <col min="25" max="25" width="14.7109375" customWidth="1"/>
     <col min="26" max="26" width="12.140625" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
@@ -472,14 +489,17 @@
         <v>22</v>
       </c>
       <c r="J4" s="5"/>
-      <c r="X4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="M4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>18</v>
@@ -494,14 +514,18 @@
       <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>7.503978762723898E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -514,16 +538,22 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="X6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>7.0270925668532852E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I6" s="6">
+        <v>3.9276656413409954E-3</v>
+      </c>
+      <c r="J6" s="6">
+        <v>2.938100784393801E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+    </row>
+    <row r="7" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <f>C6+1</f>
         <v>2</v>
@@ -538,16 +568,23 @@
         <f>H6+1</f>
         <v>2</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="X7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>7.1365854470916576E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I7" s="6">
+        <v>4.0931760176474352E-3</v>
+      </c>
+      <c r="J7" s="6">
+        <v>2.7332539099215191E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <f>M6+1</f>
+        <v>2</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+    </row>
+    <row r="8" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f t="shared" ref="C8:C55" si="0">C7+1</f>
         <v>3</v>
@@ -562,16 +599,23 @@
         <f t="shared" ref="H8:H55" si="1">H7+1</f>
         <v>3</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="X8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>5.1473346990690831E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I8" s="6">
+        <v>4.0834399209742529E-3</v>
+      </c>
+      <c r="J8" s="6">
+        <v>2.859216110827776E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" ref="M8:M55" si="2">M7+1</f>
+        <v>3</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+    </row>
+    <row r="9" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -586,16 +630,23 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="X9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>6.0591702738264662E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I9" s="6">
+        <v>3.9653085858533787E-3</v>
+      </c>
+      <c r="J9" s="6">
+        <v>3.3697382263715402E-2</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+    </row>
+    <row r="10" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -610,16 +661,23 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="X10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y10" s="3">
-        <v>8.2512322014751019E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I10" s="6">
+        <v>4.0102247051803513E-3</v>
+      </c>
+      <c r="J10" s="6">
+        <v>2.7528044971384249E-2</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+    </row>
+    <row r="11" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -634,16 +692,23 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="X11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y11" s="3">
-        <v>5.8848193825050132E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I11" s="6">
+        <v>4.034682960184212E-3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>2.9246737071336432E-2</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+    </row>
+    <row r="12" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -658,16 +723,23 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="X12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y12" s="3">
-        <v>5.777444366922288E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I12" s="6">
+        <v>4.0856080418518476E-3</v>
+      </c>
+      <c r="J12" s="6">
+        <v>2.7070889358162559E-2</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -682,16 +754,23 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="X13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y13" s="3">
-        <v>4.4363588549289151E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I13" s="6">
+        <v>4.0212399522523406E-3</v>
+      </c>
+      <c r="J13" s="6">
+        <v>3.0760583140703051E-2</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+    </row>
+    <row r="14" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -706,16 +785,23 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="X14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y14" s="3">
-        <v>6.3767118645465776E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I14" s="6">
+        <v>4.1600638428424819E-3</v>
+      </c>
+      <c r="J14" s="6">
+        <v>2.7057625430774428E-2</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+    </row>
+    <row r="15" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -730,16 +816,23 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="X15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y15" s="3">
-        <v>7.2296709713646337E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I15" s="6">
+        <v>4.1643345677634877E-3</v>
+      </c>
+      <c r="J15" s="6">
+        <v>2.8221157365190441E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+    </row>
+    <row r="16" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -754,16 +847,23 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="X16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y16" s="3">
-        <v>6.3789906383910633E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I16" s="6">
+        <v>4.1669648503705808E-3</v>
+      </c>
+      <c r="J16" s="6">
+        <v>2.746491559516968E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -778,16 +878,23 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="X17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y17" s="3">
-        <v>6.1290704209199437E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I17" s="6">
+        <v>4.207781143981207E-3</v>
+      </c>
+      <c r="J17" s="6">
+        <v>2.52225546100504E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -802,16 +909,23 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="X18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y18" s="3">
-        <v>8.0228578135459722E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I18" s="6">
+        <v>3.88392713165411E-3</v>
+      </c>
+      <c r="J18" s="6">
+        <v>3.1871663434639687E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -826,16 +940,23 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="X19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y19" s="3">
-        <v>8.6386817358361012E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I19" s="6">
+        <v>4.0208231810730704E-3</v>
+      </c>
+      <c r="J19" s="6">
+        <v>2.877508695029701E-2</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -850,10 +971,20 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I20" s="6">
+        <v>3.9667163682659207E-3</v>
+      </c>
+      <c r="J20" s="6">
+        <v>2.9584975762149919E-2</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -868,10 +999,20 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I21" s="6">
+        <v>4.0281083929292992E-3</v>
+      </c>
+      <c r="J21" s="6">
+        <v>3.0640578921422881E-2</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -886,10 +1027,20 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I22" s="6">
+        <v>3.9344421221779603E-3</v>
+      </c>
+      <c r="J22" s="6">
+        <v>3.1360408446488373E-2</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -904,10 +1055,20 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I23" s="6">
+        <v>4.033667315928525E-3</v>
+      </c>
+      <c r="J23" s="6">
+        <v>2.766472085180615E-2</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -922,10 +1083,20 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I24" s="6">
+        <v>4.0627533550975266E-3</v>
+      </c>
+      <c r="J24" s="6">
+        <v>2.8051051905327761E-2</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -940,10 +1111,20 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I25" s="6">
+        <v>4.0601247856200231E-3</v>
+      </c>
+      <c r="J25" s="6">
+        <v>2.685649943875883E-2</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -958,10 +1139,20 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I26" s="6">
+        <v>4.1440356691059043E-3</v>
+      </c>
+      <c r="J26" s="6">
+        <v>2.8275395897821829E-2</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -976,10 +1167,20 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I27" s="6">
+        <v>4.0923746968546323E-3</v>
+      </c>
+      <c r="J27" s="6">
+        <v>2.9491834694450731E-2</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -994,10 +1195,20 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I28" s="6">
+        <v>4.0092400337476226E-3</v>
+      </c>
+      <c r="J28" s="6">
+        <v>2.7938694317027651E-2</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1012,10 +1223,20 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I29" s="6">
+        <v>4.0607467404597773E-3</v>
+      </c>
+      <c r="J29" s="6">
+        <v>2.8110171562992531E-2</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1030,10 +1251,20 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I30" s="6">
+        <v>4.1337080155582464E-3</v>
+      </c>
+      <c r="J30" s="6">
+        <v>2.8244668368679591E-2</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1048,10 +1279,20 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I31" s="6">
+        <v>4.0222332460388421E-3</v>
+      </c>
+      <c r="J31" s="6">
+        <v>2.9979743155205862E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1066,10 +1307,20 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I32" s="6">
+        <v>3.9435417797970213E-3</v>
+      </c>
+      <c r="J32" s="6">
+        <v>2.883445790932581E-2</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1084,10 +1335,20 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="6">
+        <v>4.0476213611508804E-3</v>
+      </c>
+      <c r="J33" s="6">
+        <v>2.9723694880079012E-2</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1102,10 +1363,20 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="6">
+        <v>3.971880002067339E-3</v>
+      </c>
+      <c r="J34" s="6">
+        <v>3.2181297726158173E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1120,10 +1391,20 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="6">
+        <v>4.1353344065271592E-3</v>
+      </c>
+      <c r="J35" s="6">
+        <v>2.6668192381769339E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1138,10 +1419,20 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="6">
+        <v>4.1260087831707206E-3</v>
+      </c>
+      <c r="J36" s="6">
+        <v>2.572842267652619E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1156,10 +1447,20 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="6">
+        <v>4.169653887626453E-3</v>
+      </c>
+      <c r="J37" s="6">
+        <v>2.498112175892889E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1174,10 +1475,20 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="6">
+        <v>4.0945780755847431E-3</v>
+      </c>
+      <c r="J38" s="6">
+        <v>2.912116071864683E-2</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1192,10 +1503,20 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="6">
+        <v>3.8959106702949999E-3</v>
+      </c>
+      <c r="J39" s="6">
+        <v>2.9522497118318371E-2</v>
+      </c>
+      <c r="M39" s="1">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1210,10 +1531,20 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="6">
+        <v>4.1078543061923998E-3</v>
+      </c>
+      <c r="J40" s="6">
+        <v>2.7361907552202649E-2</v>
+      </c>
+      <c r="M40" s="1">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1228,10 +1559,20 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="6">
+        <v>4.0614300469087958E-3</v>
+      </c>
+      <c r="J41" s="6">
+        <v>2.7770528645042439E-2</v>
+      </c>
+      <c r="M41" s="1">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1246,10 +1587,20 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="6">
+        <v>4.0649979498831104E-3</v>
+      </c>
+      <c r="J42" s="6">
+        <v>2.9784363038674121E-2</v>
+      </c>
+      <c r="M42" s="1">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1264,10 +1615,20 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="6">
+        <v>4.1283587959996624E-3</v>
+      </c>
+      <c r="J43" s="6">
+        <v>2.6708192012520969E-2</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1282,10 +1643,20 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I44" s="6">
+        <v>4.0722251071869204E-3</v>
+      </c>
+      <c r="J44" s="6">
+        <v>2.9642513860646261E-2</v>
+      </c>
+      <c r="M44" s="1">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1300,10 +1671,20 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I45" s="6">
+        <v>4.0901595646759279E-3</v>
+      </c>
+      <c r="J45" s="6">
+        <v>2.723870153452692E-2</v>
+      </c>
+      <c r="M45" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1318,10 +1699,20 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I46" s="6">
+        <v>4.0454915078177384E-3</v>
+      </c>
+      <c r="J46" s="6">
+        <v>2.7564969143087679E-2</v>
+      </c>
+      <c r="M46" s="1">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1336,10 +1727,20 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I47" s="6">
+        <v>3.9399892864224097E-3</v>
+      </c>
+      <c r="J47" s="6">
+        <v>2.965372102676064E-2</v>
+      </c>
+      <c r="M47" s="1">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1354,10 +1755,20 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I48" s="6">
+        <v>3.9380767657326479E-3</v>
+      </c>
+      <c r="J48" s="6">
+        <v>2.8566517870036268E-2</v>
+      </c>
+      <c r="M48" s="1">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1372,10 +1783,20 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="6">
+        <v>4.1488357471704523E-3</v>
+      </c>
+      <c r="J49" s="6">
+        <v>2.988827595953647E-2</v>
+      </c>
+      <c r="M49" s="1">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1390,10 +1811,20 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="6">
+        <v>4.0823180508569642E-3</v>
+      </c>
+      <c r="J50" s="6">
+        <v>2.9601519781782541E-2</v>
+      </c>
+      <c r="M50" s="1">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1408,10 +1839,20 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="6">
+        <v>3.9773714885452749E-3</v>
+      </c>
+      <c r="J51" s="6">
+        <v>3.0137090798804968E-2</v>
+      </c>
+      <c r="M51" s="1">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1426,10 +1867,20 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="6">
+        <v>4.0884666895494798E-3</v>
+      </c>
+      <c r="J52" s="6">
+        <v>2.6940496182122121E-2</v>
+      </c>
+      <c r="M52" s="1">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1444,10 +1895,20 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="6">
+        <v>4.0124895663203076E-3</v>
+      </c>
+      <c r="J53" s="6">
+        <v>2.793593832506891E-2</v>
+      </c>
+      <c r="M53" s="1">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1462,10 +1923,20 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="6">
+        <v>4.0316403449870289E-3</v>
+      </c>
+      <c r="J54" s="6">
+        <v>2.674363132379649E-2</v>
+      </c>
+      <c r="M54" s="1">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1480,16 +1951,28 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I55" s="6">
+        <v>4.0731463801027728E-3</v>
+      </c>
+      <c r="J55" s="6">
+        <v>2.7440350501594851E-2</v>
+      </c>
+      <c r="M55" s="1">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>20</v>
       </c>
@@ -1504,16 +1987,27 @@
       <c r="H57" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I57" s="6" t="e">
+      <c r="I57" s="6">
         <f>AVERAGE(I6:I55)</f>
+        <v>4.0524154369865045E-3</v>
+      </c>
+      <c r="J57" s="6">
+        <f>AVERAGE(J6:J55)</f>
+        <v>2.8563213085818856E-2</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N57" s="6" t="e">
+        <f>AVERAGE(N6:N55)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J57" s="6" t="e">
-        <f>AVERAGE(J6:J55)</f>
+      <c r="O57" s="6" t="e">
+        <f>AVERAGE(O6:O55)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>21</v>
       </c>
@@ -1528,13 +2022,230 @@
       <c r="H58" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I58" s="6" t="e">
+      <c r="I58" s="6">
         <f>_xlfn.STDEV.S(I6:I55)</f>
+        <v>7.6854460905943545E-5</v>
+      </c>
+      <c r="J58" s="6">
+        <f>_xlfn.STDEV.S(J6:J55)</f>
+        <v>1.7432818564365002E-3</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N58" s="6" t="e">
+        <f>_xlfn.STDEV.S(N6:N55)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J58" s="6" t="e">
-        <f>_xlfn.STDEV.S(J6:J55)</f>
+      <c r="O58" s="6" t="e">
+        <f>_xlfn.STDEV.S(O6:O55)</f>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.503978762723898E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6.3792487189086589E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.0270925668532852E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.3428122590238228E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.1365854470916576E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5.8729321315472302E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5.1473346990690831E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5.5122800816895447E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6.0591702738264662E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6.2159460138943377E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8.2512322014751019E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6.9456315592393084E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.8848193825050132E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.3472015861343753E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5.777444366922288E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6.8587388082312711E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4.4363588549289151E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5.0642202227123838E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>6.3767118645465776E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8.3471995894845372E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7.2296709713646337E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>7.1226425486352468E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>6.3789906383910633E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6.0042637869732782E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>6.1290704209199437E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6.7099820093954946E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>8.0228578135459722E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>9.6276674432277998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8.6386817358361012E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7.6492332409027031E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-16 for interregional saldo
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-16.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-16.xlsx
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V43" sqref="V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,8 +547,12 @@
       <c r="M6" s="1">
         <v>1</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="N6" s="6">
+        <v>4.7695003077224078E-3</v>
+      </c>
+      <c r="O6" s="6">
+        <v>3.118292825736188E-2</v>
+      </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
@@ -578,8 +582,12 @@
         <f>M6+1</f>
         <v>2</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="N7" s="6">
+        <v>4.5720456292513336E-3</v>
+      </c>
+      <c r="O7" s="6">
+        <v>3.3525868579185748E-2</v>
+      </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -609,8 +617,12 @@
         <f t="shared" ref="M8:M55" si="2">M7+1</f>
         <v>3</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="N8" s="6">
+        <v>4.5515442489738557E-3</v>
+      </c>
+      <c r="O8" s="6">
+        <v>3.3755682566183873E-2</v>
+      </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
@@ -640,8 +652,12 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="N9" s="6">
+        <v>4.6259677353847383E-3</v>
+      </c>
+      <c r="O9" s="6">
+        <v>3.3223096939218863E-2</v>
+      </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -671,8 +687,12 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="N10" s="6">
+        <v>4.5361807639645356E-3</v>
+      </c>
+      <c r="O10" s="6">
+        <v>3.1339850159775147E-2</v>
+      </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
@@ -702,8 +722,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="N11" s="6">
+        <v>4.5716462394260133E-3</v>
+      </c>
+      <c r="O11" s="6">
+        <v>3.5131207937474568E-2</v>
+      </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
@@ -733,8 +757,12 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="N12" s="6">
+        <v>4.5960000125573894E-3</v>
+      </c>
+      <c r="O12" s="6">
+        <v>3.3711821218537587E-2</v>
+      </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
@@ -764,8 +792,12 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+      <c r="N13" s="6">
+        <v>4.6727769605473214E-3</v>
+      </c>
+      <c r="O13" s="6">
+        <v>3.3532651304816641E-2</v>
+      </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -795,8 +827,12 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="N14" s="6">
+        <v>4.5249634270531636E-3</v>
+      </c>
+      <c r="O14" s="6">
+        <v>3.8052163397268322E-2</v>
+      </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
@@ -826,8 +862,12 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="N15" s="6">
+        <v>4.6851858352022907E-3</v>
+      </c>
+      <c r="O15" s="6">
+        <v>2.95066706798136E-2</v>
+      </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
@@ -857,8 +897,12 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="N16" s="6">
+        <v>4.6711126068756043E-3</v>
+      </c>
+      <c r="O16" s="6">
+        <v>3.1890609473540422E-2</v>
+      </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -888,8 +932,12 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
+      <c r="N17" s="6">
+        <v>4.595814503362672E-3</v>
+      </c>
+      <c r="O17" s="6">
+        <v>3.1479945387102873E-2</v>
+      </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
@@ -919,8 +967,12 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
+      <c r="N18" s="6">
+        <v>4.5985444195138928E-3</v>
+      </c>
+      <c r="O18" s="6">
+        <v>3.2261766252048477E-2</v>
+      </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
@@ -950,8 +1002,12 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="N19" s="6">
+        <v>4.6672749040183176E-3</v>
+      </c>
+      <c r="O19" s="6">
+        <v>3.1205521975054051E-2</v>
+      </c>
       <c r="X19" s="4"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -981,8 +1037,12 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
+      <c r="N20" s="6">
+        <v>4.6756312767027566E-3</v>
+      </c>
+      <c r="O20" s="6">
+        <v>3.0543567477029351E-2</v>
+      </c>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
@@ -1009,8 +1069,12 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
+      <c r="N21" s="6">
+        <v>4.7327213927244594E-3</v>
+      </c>
+      <c r="O21" s="6">
+        <v>3.4007994157639679E-2</v>
+      </c>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
@@ -1037,8 +1101,12 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="N22" s="6">
+        <v>4.6599265795111587E-3</v>
+      </c>
+      <c r="O22" s="6">
+        <v>3.2751649259127082E-2</v>
+      </c>
     </row>
     <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
@@ -1065,8 +1133,12 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="N23" s="6">
+        <v>4.4404871608199259E-3</v>
+      </c>
+      <c r="O23" s="6">
+        <v>3.7258792699951603E-2</v>
+      </c>
     </row>
     <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
@@ -1093,8 +1165,12 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
+      <c r="N24" s="6">
+        <v>4.6850595714198551E-3</v>
+      </c>
+      <c r="O24" s="6">
+        <v>3.3063752032043793E-2</v>
+      </c>
     </row>
     <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
@@ -1121,8 +1197,12 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
+      <c r="N25" s="6">
+        <v>4.5944024860740213E-3</v>
+      </c>
+      <c r="O25" s="6">
+        <v>3.186562841467093E-2</v>
+      </c>
     </row>
     <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
@@ -1149,8 +1229,12 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="N26" s="6">
+        <v>4.7206878161942306E-3</v>
+      </c>
+      <c r="O26" s="6">
+        <v>3.0976917866293009E-2</v>
+      </c>
     </row>
     <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
@@ -1177,8 +1261,12 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
+      <c r="N27" s="6">
+        <v>4.6768410862040814E-3</v>
+      </c>
+      <c r="O27" s="6">
+        <v>3.1723597198414458E-2</v>
+      </c>
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
@@ -1205,8 +1293,12 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
+      <c r="N28" s="6">
+        <v>4.6595010932994826E-3</v>
+      </c>
+      <c r="O28" s="6">
+        <v>3.1633979506510833E-2</v>
+      </c>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
@@ -1233,8 +1325,12 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
+      <c r="N29" s="6">
+        <v>4.6488932782003346E-3</v>
+      </c>
+      <c r="O29" s="6">
+        <v>3.5018188400716688E-2</v>
+      </c>
     </row>
     <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
@@ -1261,8 +1357,12 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
+      <c r="N30" s="6">
+        <v>4.4754589531873293E-3</v>
+      </c>
+      <c r="O30" s="6">
+        <v>3.5571871154928172E-2</v>
+      </c>
     </row>
     <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
@@ -1289,8 +1389,12 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
+      <c r="N31" s="6">
+        <v>4.8468629148511293E-3</v>
+      </c>
+      <c r="O31" s="6">
+        <v>2.9428253484147342E-2</v>
+      </c>
     </row>
     <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
@@ -1317,8 +1421,12 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
+      <c r="N32" s="6">
+        <v>4.5299699096176338E-3</v>
+      </c>
+      <c r="O32" s="6">
+        <v>3.3993385068867177E-2</v>
+      </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
@@ -1345,8 +1453,12 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
+      <c r="N33" s="6">
+        <v>4.4468747734298332E-3</v>
+      </c>
+      <c r="O33" s="6">
+        <v>3.5616620067012897E-2</v>
+      </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
@@ -1373,8 +1485,12 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
+      <c r="N34" s="6">
+        <v>4.6087905955834573E-3</v>
+      </c>
+      <c r="O34" s="6">
+        <v>3.427787405639296E-2</v>
+      </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
@@ -1401,8 +1517,12 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
+      <c r="N35" s="6">
+        <v>4.560760129113382E-3</v>
+      </c>
+      <c r="O35" s="6">
+        <v>3.1577120832329247E-2</v>
+      </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
@@ -1429,8 +1549,12 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
+      <c r="N36" s="6">
+        <v>4.5141551074862566E-3</v>
+      </c>
+      <c r="O36" s="6">
+        <v>3.568596345990286E-2</v>
+      </c>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
@@ -1457,8 +1581,12 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
+      <c r="N37" s="6">
+        <v>4.5930025186855317E-3</v>
+      </c>
+      <c r="O37" s="6">
+        <v>3.3605636319693898E-2</v>
+      </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
@@ -1485,8 +1613,12 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
+      <c r="N38" s="6">
+        <v>4.5747805887478774E-3</v>
+      </c>
+      <c r="O38" s="6">
+        <v>2.9587805335058889E-2</v>
+      </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
@@ -1513,8 +1645,12 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
+      <c r="N39" s="6">
+        <v>4.5343388878611914E-3</v>
+      </c>
+      <c r="O39" s="6">
+        <v>3.4012705798304579E-2</v>
+      </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
@@ -1541,8 +1677,12 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
+      <c r="N40" s="6">
+        <v>4.6604170580406574E-3</v>
+      </c>
+      <c r="O40" s="6">
+        <v>3.1516542249970768E-2</v>
+      </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
@@ -1569,8 +1709,12 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
+      <c r="N41" s="6">
+        <v>4.623230705287292E-3</v>
+      </c>
+      <c r="O41" s="6">
+        <v>3.118880653929898E-2</v>
+      </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
@@ -1597,8 +1741,12 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
+      <c r="N42" s="6">
+        <v>4.6227011351756987E-3</v>
+      </c>
+      <c r="O42" s="6">
+        <v>3.5455802631071648E-2</v>
+      </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
@@ -1625,8 +1773,12 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
+      <c r="N43" s="6">
+        <v>4.6537650321949384E-3</v>
+      </c>
+      <c r="O43" s="6">
+        <v>3.2489236391748243E-2</v>
+      </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
@@ -1653,8 +1805,12 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
+      <c r="N44" s="6">
+        <v>4.6426568961247224E-3</v>
+      </c>
+      <c r="O44" s="6">
+        <v>3.341286040584953E-2</v>
+      </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
@@ -1681,8 +1837,12 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
+      <c r="N45" s="6">
+        <v>4.4332302146524944E-3</v>
+      </c>
+      <c r="O45" s="6">
+        <v>3.8752375060404833E-2</v>
+      </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
@@ -1709,8 +1869,12 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
+      <c r="N46" s="6">
+        <v>4.673619534517324E-3</v>
+      </c>
+      <c r="O46" s="6">
+        <v>2.936176879549791E-2</v>
+      </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
@@ -1737,8 +1901,12 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
+      <c r="N47" s="6">
+        <v>4.5802204049157176E-3</v>
+      </c>
+      <c r="O47" s="6">
+        <v>3.2698903014279683E-2</v>
+      </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
@@ -1765,8 +1933,12 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
+      <c r="N48" s="6">
+        <v>4.7043106275732986E-3</v>
+      </c>
+      <c r="O48" s="6">
+        <v>3.0282751698742449E-2</v>
+      </c>
     </row>
     <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
@@ -1793,8 +1965,12 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
+      <c r="N49" s="6">
+        <v>4.6604296739450992E-3</v>
+      </c>
+      <c r="O49" s="6">
+        <v>3.2144299105788747E-2</v>
+      </c>
     </row>
     <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
@@ -1821,8 +1997,12 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
+      <c r="N50" s="6">
+        <v>4.5346488444017114E-3</v>
+      </c>
+      <c r="O50" s="6">
+        <v>3.6354363943475479E-2</v>
+      </c>
     </row>
     <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
@@ -1849,8 +2029,12 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
+      <c r="N51" s="6">
+        <v>4.5783474977289414E-3</v>
+      </c>
+      <c r="O51" s="6">
+        <v>3.1746551808347588E-2</v>
+      </c>
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
@@ -1877,8 +2061,12 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
+      <c r="N52" s="6">
+        <v>4.6121546506134106E-3</v>
+      </c>
+      <c r="O52" s="6">
+        <v>3.3317772709260049E-2</v>
+      </c>
     </row>
     <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
@@ -1905,8 +2093,12 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
+      <c r="N53" s="6">
+        <v>4.4702526660844004E-3</v>
+      </c>
+      <c r="O53" s="6">
+        <v>3.5742529622319587E-2</v>
+      </c>
     </row>
     <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
@@ -1933,8 +2125,12 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
+      <c r="N54" s="6">
+        <v>4.694499494012701E-3</v>
+      </c>
+      <c r="O54" s="6">
+        <v>3.1921624442287702E-2</v>
+      </c>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
@@ -1961,8 +2157,12 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
+      <c r="N55" s="6">
+        <v>4.4949919681506788E-3</v>
+      </c>
+      <c r="O55" s="6">
+        <v>3.359791864684826E-2</v>
+      </c>
     </row>
     <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D56" s="7"/>
@@ -1998,13 +2198,13 @@
       <c r="M57" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N57" s="6" t="e">
+      <c r="N57" s="6">
         <f>AVERAGE(N6:N55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O57" s="6" t="e">
+        <v>4.6091436023397315E-3</v>
+      </c>
+      <c r="O57" s="6">
         <f>AVERAGE(O6:O55)</f>
-        <v>#DIV/0!</v>
+        <v>3.3039703875632175E-2</v>
       </c>
     </row>
     <row r="58" spans="3:15" x14ac:dyDescent="0.25">
@@ -2033,13 +2233,13 @@
       <c r="M58" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N58" s="6" t="e">
+      <c r="N58" s="6">
         <f>_xlfn.STDEV.S(N6:N55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O58" s="6" t="e">
+        <v>8.6320087022079321E-5</v>
+      </c>
+      <c r="O58" s="6">
         <f>_xlfn.STDEV.S(O6:O55)</f>
-        <v>#DIV/0!</v>
+        <v>2.189953442958352E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2053,7 +2253,7 @@
   <dimension ref="C4:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,6 +2293,9 @@
       <c r="E5" s="3">
         <v>6.3792487189086589E-2</v>
       </c>
+      <c r="F5" s="3">
+        <v>8.8413027272881861E-2</v>
+      </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -2104,6 +2307,9 @@
       <c r="E6" s="3">
         <v>5.3428122590238228E-2</v>
       </c>
+      <c r="F6" s="3">
+        <v>0.13328645042113921</v>
+      </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -2115,6 +2321,9 @@
       <c r="E7" s="3">
         <v>5.8729321315472302E-2</v>
       </c>
+      <c r="F7" s="3">
+        <v>7.9719945271623127E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -2126,6 +2335,9 @@
       <c r="E8" s="3">
         <v>5.5122800816895447E-2</v>
       </c>
+      <c r="F8" s="3">
+        <v>6.058922124692831E-2</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -2137,6 +2349,9 @@
       <c r="E9" s="3">
         <v>6.2159460138943377E-2</v>
       </c>
+      <c r="F9" s="3">
+        <v>5.6071573053039482E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
@@ -2148,6 +2363,9 @@
       <c r="E10" s="3">
         <v>6.9456315592393084E-2</v>
       </c>
+      <c r="F10" s="3">
+        <v>6.6070805140619762E-2</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
@@ -2159,6 +2377,9 @@
       <c r="E11" s="3">
         <v>6.3472015861343753E-2</v>
       </c>
+      <c r="F11" s="3">
+        <v>5.5571882969546488E-2</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
@@ -2170,6 +2391,9 @@
       <c r="E12" s="3">
         <v>6.8587388082312711E-2</v>
       </c>
+      <c r="F12" s="3">
+        <v>5.3242116681780208E-2</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -2181,6 +2405,9 @@
       <c r="E13" s="3">
         <v>5.0642202227123838E-2</v>
       </c>
+      <c r="F13" s="3">
+        <v>5.3475660887844681E-2</v>
+      </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
@@ -2192,6 +2419,9 @@
       <c r="E14" s="3">
         <v>8.3471995894845372E-2</v>
       </c>
+      <c r="F14" s="3">
+        <v>5.7848632447795943E-2</v>
+      </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -2203,6 +2433,9 @@
       <c r="E15" s="3">
         <v>7.1226425486352468E-2</v>
       </c>
+      <c r="F15" s="3">
+        <v>6.580257898426678E-2</v>
+      </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
@@ -2214,8 +2447,11 @@
       <c r="E16" s="3">
         <v>6.0042637869732782E-2</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <v>6.0617071528018117E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2225,8 +2461,11 @@
       <c r="E17" s="3">
         <v>6.7099820093954946E-2</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="3">
+        <v>6.6874939593002225E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2236,8 +2475,11 @@
       <c r="E18" s="3">
         <v>9.6276674432277998E-2</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="3">
+        <v>3.7055712634370012E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2247,8 +2489,12 @@
       <c r="E19" s="3">
         <v>7.6492332409027031E-2</v>
       </c>
+      <c r="F19" s="3">
+        <v>6.5360381867143935E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test-16 for international saldo
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-16.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-16.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mse (unbalanced set)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>features</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24 interreg.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 internat.csv)</t>
   </si>
 </sst>
 </file>
@@ -461,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V43" sqref="V43"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,6 +476,8 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
     <col min="24" max="24" width="17.7109375" customWidth="1"/>
     <col min="25" max="25" width="14.7109375" customWidth="1"/>
     <col min="26" max="26" width="12.140625" customWidth="1"/>
@@ -493,6 +498,10 @@
         <v>26</v>
       </c>
       <c r="O4" s="5"/>
+      <c r="R4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="5"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -521,6 +530,13 @@
       <c r="O5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
@@ -552,6 +568,15 @@
       </c>
       <c r="O6" s="6">
         <v>3.118292825736188E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="6">
+        <v>4.3464136345046341E-3</v>
+      </c>
+      <c r="T6" s="6">
+        <v>3.116807114836714E-2</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="3"/>
@@ -588,6 +613,16 @@
       <c r="O7" s="6">
         <v>3.3525868579185748E-2</v>
       </c>
+      <c r="R7" s="1">
+        <f>R6+1</f>
+        <v>2</v>
+      </c>
+      <c r="S7" s="6">
+        <v>4.1322322944861564E-3</v>
+      </c>
+      <c r="T7" s="6">
+        <v>3.3054643014229813E-2</v>
+      </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -623,6 +658,16 @@
       <c r="O8" s="6">
         <v>3.3755682566183873E-2</v>
       </c>
+      <c r="R8" s="1">
+        <f t="shared" ref="R8:R55" si="3">R7+1</f>
+        <v>3</v>
+      </c>
+      <c r="S8" s="6">
+        <v>4.245986127271696E-3</v>
+      </c>
+      <c r="T8" s="6">
+        <v>3.108383898615092E-2</v>
+      </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
@@ -658,6 +703,16 @@
       <c r="O9" s="6">
         <v>3.3223096939218863E-2</v>
       </c>
+      <c r="R9" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S9" s="6">
+        <v>4.3051286430780683E-3</v>
+      </c>
+      <c r="T9" s="6">
+        <v>3.0194434171019972E-2</v>
+      </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -693,6 +748,16 @@
       <c r="O10" s="6">
         <v>3.1339850159775147E-2</v>
       </c>
+      <c r="R10" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S10" s="6">
+        <v>4.3883287635906789E-3</v>
+      </c>
+      <c r="T10" s="6">
+        <v>2.8288279560781129E-2</v>
+      </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
@@ -728,6 +793,16 @@
       <c r="O11" s="6">
         <v>3.5131207937474568E-2</v>
       </c>
+      <c r="R11" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S11" s="6">
+        <v>4.1644627068813207E-3</v>
+      </c>
+      <c r="T11" s="6">
+        <v>2.979760117720244E-2</v>
+      </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
@@ -763,6 +838,16 @@
       <c r="O12" s="6">
         <v>3.3711821218537587E-2</v>
       </c>
+      <c r="R12" s="1">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S12" s="6">
+        <v>4.4063095816940243E-3</v>
+      </c>
+      <c r="T12" s="6">
+        <v>2.7917470658922441E-2</v>
+      </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
@@ -798,6 +883,16 @@
       <c r="O13" s="6">
         <v>3.3532651304816641E-2</v>
       </c>
+      <c r="R13" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S13" s="6">
+        <v>4.305360452574453E-3</v>
+      </c>
+      <c r="T13" s="6">
+        <v>3.0519832188945769E-2</v>
+      </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -833,6 +928,16 @@
       <c r="O14" s="6">
         <v>3.8052163397268322E-2</v>
       </c>
+      <c r="R14" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S14" s="6">
+        <v>4.0600328619609348E-3</v>
+      </c>
+      <c r="T14" s="6">
+        <v>3.4080878090518109E-2</v>
+      </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
@@ -868,6 +973,16 @@
       <c r="O15" s="6">
         <v>2.95066706798136E-2</v>
       </c>
+      <c r="R15" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S15" s="6">
+        <v>4.4606921492969373E-3</v>
+      </c>
+      <c r="T15" s="6">
+        <v>2.7905839009573719E-2</v>
+      </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
@@ -903,6 +1018,16 @@
       <c r="O16" s="6">
         <v>3.1890609473540422E-2</v>
       </c>
+      <c r="R16" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S16" s="6">
+        <v>4.3512747802332691E-3</v>
+      </c>
+      <c r="T16" s="6">
+        <v>3.031577346109323E-2</v>
+      </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -938,6 +1063,16 @@
       <c r="O17" s="6">
         <v>3.1479945387102873E-2</v>
       </c>
+      <c r="R17" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S17" s="6">
+        <v>4.4375255107605956E-3</v>
+      </c>
+      <c r="T17" s="6">
+        <v>2.676486437577889E-2</v>
+      </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
@@ -973,6 +1108,16 @@
       <c r="O18" s="6">
         <v>3.2261766252048477E-2</v>
       </c>
+      <c r="R18" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S18" s="6">
+        <v>4.101801677302226E-3</v>
+      </c>
+      <c r="T18" s="6">
+        <v>3.244302216049625E-2</v>
+      </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
@@ -1008,6 +1153,16 @@
       <c r="O19" s="6">
         <v>3.1205521975054051E-2</v>
       </c>
+      <c r="R19" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S19" s="6">
+        <v>4.327883429768681E-3</v>
+      </c>
+      <c r="T19" s="6">
+        <v>2.742230231718101E-2</v>
+      </c>
       <c r="X19" s="4"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -1043,6 +1198,16 @@
       <c r="O20" s="6">
         <v>3.0543567477029351E-2</v>
       </c>
+      <c r="R20" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S20" s="6">
+        <v>4.2633680390361658E-3</v>
+      </c>
+      <c r="T20" s="6">
+        <v>3.0970338565573852E-2</v>
+      </c>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
@@ -1075,6 +1240,16 @@
       <c r="O21" s="6">
         <v>3.4007994157639679E-2</v>
       </c>
+      <c r="R21" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S21" s="6">
+        <v>4.2649931851129266E-3</v>
+      </c>
+      <c r="T21" s="6">
+        <v>2.9165090937649189E-2</v>
+      </c>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
@@ -1107,6 +1282,16 @@
       <c r="O22" s="6">
         <v>3.2751649259127082E-2</v>
       </c>
+      <c r="R22" s="1">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S22" s="6">
+        <v>4.2020821490466346E-3</v>
+      </c>
+      <c r="T22" s="6">
+        <v>3.1553740740358008E-2</v>
+      </c>
     </row>
     <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
@@ -1139,6 +1324,16 @@
       <c r="O23" s="6">
         <v>3.7258792699951603E-2</v>
       </c>
+      <c r="R23" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S23" s="6">
+        <v>4.0915455919091218E-3</v>
+      </c>
+      <c r="T23" s="6">
+        <v>3.222157557102838E-2</v>
+      </c>
     </row>
     <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
@@ -1171,6 +1366,16 @@
       <c r="O24" s="6">
         <v>3.3063752032043793E-2</v>
       </c>
+      <c r="R24" s="1">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S24" s="6">
+        <v>4.2019406861181557E-3</v>
+      </c>
+      <c r="T24" s="6">
+        <v>3.4338513514612028E-2</v>
+      </c>
     </row>
     <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
@@ -1203,6 +1408,16 @@
       <c r="O25" s="6">
         <v>3.186562841467093E-2</v>
       </c>
+      <c r="R25" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S25" s="6">
+        <v>4.1731735519369619E-3</v>
+      </c>
+      <c r="T25" s="6">
+        <v>3.078533535596114E-2</v>
+      </c>
     </row>
     <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
@@ -1235,6 +1450,16 @@
       <c r="O26" s="6">
         <v>3.0976917866293009E-2</v>
       </c>
+      <c r="R26" s="1">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S26" s="6">
+        <v>4.1749451169314474E-3</v>
+      </c>
+      <c r="T26" s="6">
+        <v>3.2811608964135777E-2</v>
+      </c>
     </row>
     <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
@@ -1267,6 +1492,16 @@
       <c r="O27" s="6">
         <v>3.1723597198414458E-2</v>
       </c>
+      <c r="R27" s="1">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S27" s="6">
+        <v>4.1372000924971026E-3</v>
+      </c>
+      <c r="T27" s="6">
+        <v>3.2087318229300499E-2</v>
+      </c>
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
@@ -1299,6 +1534,16 @@
       <c r="O28" s="6">
         <v>3.1633979506510833E-2</v>
       </c>
+      <c r="R28" s="1">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S28" s="6">
+        <v>4.2147154540659332E-3</v>
+      </c>
+      <c r="T28" s="6">
+        <v>3.2973092194213599E-2</v>
+      </c>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
@@ -1331,6 +1576,16 @@
       <c r="O29" s="6">
         <v>3.5018188400716688E-2</v>
       </c>
+      <c r="R29" s="1">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S29" s="6">
+        <v>4.3283179080407033E-3</v>
+      </c>
+      <c r="T29" s="6">
+        <v>2.8671149456533599E-2</v>
+      </c>
     </row>
     <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
@@ -1363,6 +1618,16 @@
       <c r="O30" s="6">
         <v>3.5571871154928172E-2</v>
       </c>
+      <c r="R30" s="1">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S30" s="6">
+        <v>4.2247888583703567E-3</v>
+      </c>
+      <c r="T30" s="6">
+        <v>3.0273698786905549E-2</v>
+      </c>
     </row>
     <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
@@ -1395,6 +1660,16 @@
       <c r="O31" s="6">
         <v>2.9428253484147342E-2</v>
       </c>
+      <c r="R31" s="1">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S31" s="6">
+        <v>4.3553806903342601E-3</v>
+      </c>
+      <c r="T31" s="6">
+        <v>2.7265348507634572E-2</v>
+      </c>
     </row>
     <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
@@ -1427,8 +1702,18 @@
       <c r="O32" s="6">
         <v>3.3993385068867177E-2</v>
       </c>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R32" s="1">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S32" s="6">
+        <v>4.3997969413036072E-3</v>
+      </c>
+      <c r="T32" s="6">
+        <v>2.7512598977066548E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1459,8 +1744,18 @@
       <c r="O33" s="6">
         <v>3.5616620067012897E-2</v>
       </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R33" s="1">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S33" s="6">
+        <v>4.2740886592076534E-3</v>
+      </c>
+      <c r="T33" s="6">
+        <v>2.833357080196228E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1491,8 +1786,18 @@
       <c r="O34" s="6">
         <v>3.427787405639296E-2</v>
       </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R34" s="1">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S34" s="6">
+        <v>4.3099104114582504E-3</v>
+      </c>
+      <c r="T34" s="6">
+        <v>3.0821348940267491E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1523,8 +1828,18 @@
       <c r="O35" s="6">
         <v>3.1577120832329247E-2</v>
       </c>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R35" s="1">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S35" s="6">
+        <v>4.2714999539581206E-3</v>
+      </c>
+      <c r="T35" s="6">
+        <v>3.3114456461260169E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1555,8 +1870,18 @@
       <c r="O36" s="6">
         <v>3.568596345990286E-2</v>
       </c>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R36" s="1">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S36" s="6">
+        <v>4.1180521793424208E-3</v>
+      </c>
+      <c r="T36" s="6">
+        <v>3.0147748646701712E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1587,8 +1912,18 @@
       <c r="O37" s="6">
         <v>3.3605636319693898E-2</v>
       </c>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R37" s="1">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S37" s="6">
+        <v>4.2776355763421443E-3</v>
+      </c>
+      <c r="T37" s="6">
+        <v>2.9347841713299849E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1619,8 +1954,18 @@
       <c r="O38" s="6">
         <v>2.9587805335058889E-2</v>
       </c>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R38" s="1">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S38" s="6">
+        <v>4.2243375273926234E-3</v>
+      </c>
+      <c r="T38" s="6">
+        <v>2.9967055774512821E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1651,8 +1996,18 @@
       <c r="O39" s="6">
         <v>3.4012705798304579E-2</v>
       </c>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R39" s="1">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S39" s="6">
+        <v>4.2998733717421354E-3</v>
+      </c>
+      <c r="T39" s="6">
+        <v>3.0381360378861511E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1683,8 +2038,18 @@
       <c r="O40" s="6">
         <v>3.1516542249970768E-2</v>
       </c>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R40" s="1">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S40" s="6">
+        <v>4.3399854466326391E-3</v>
+      </c>
+      <c r="T40" s="6">
+        <v>3.0720402750020609E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1715,8 +2080,18 @@
       <c r="O41" s="6">
         <v>3.118880653929898E-2</v>
       </c>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R41" s="1">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S41" s="6">
+        <v>4.1204651763794356E-3</v>
+      </c>
+      <c r="T41" s="6">
+        <v>3.2751144696652898E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1747,8 +2122,18 @@
       <c r="O42" s="6">
         <v>3.5455802631071648E-2</v>
       </c>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R42" s="1">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S42" s="6">
+        <v>4.1164986250585862E-3</v>
+      </c>
+      <c r="T42" s="6">
+        <v>3.4187147659866933E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1779,8 +2164,18 @@
       <c r="O43" s="6">
         <v>3.2489236391748243E-2</v>
       </c>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R43" s="1">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S43" s="6">
+        <v>4.1253775411156284E-3</v>
+      </c>
+      <c r="T43" s="6">
+        <v>3.1461513549286967E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1811,8 +2206,18 @@
       <c r="O44" s="6">
         <v>3.341286040584953E-2</v>
       </c>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R44" s="1">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S44" s="6">
+        <v>4.3007640099928107E-3</v>
+      </c>
+      <c r="T44" s="6">
+        <v>2.7646315652562689E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1843,8 +2248,18 @@
       <c r="O45" s="6">
         <v>3.8752375060404833E-2</v>
       </c>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R45" s="1">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S45" s="6">
+        <v>4.1395341413740594E-3</v>
+      </c>
+      <c r="T45" s="6">
+        <v>3.1726740976652748E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1875,8 +2290,18 @@
       <c r="O46" s="6">
         <v>2.936176879549791E-2</v>
       </c>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R46" s="1">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S46" s="6">
+        <v>4.1302392643770636E-3</v>
+      </c>
+      <c r="T46" s="6">
+        <v>3.2546724006603377E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1907,8 +2332,18 @@
       <c r="O47" s="6">
         <v>3.2698903014279683E-2</v>
       </c>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R47" s="1">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S47" s="6">
+        <v>4.184841667372795E-3</v>
+      </c>
+      <c r="T47" s="6">
+        <v>3.2192799114342537E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1939,8 +2374,18 @@
       <c r="O48" s="6">
         <v>3.0282751698742449E-2</v>
       </c>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R48" s="1">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S48" s="6">
+        <v>4.3719658006430243E-3</v>
+      </c>
+      <c r="T48" s="6">
+        <v>2.8386630958376069E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1971,8 +2416,18 @@
       <c r="O49" s="6">
         <v>3.2144299105788747E-2</v>
       </c>
-    </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R49" s="1">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S49" s="6">
+        <v>4.3330919572299662E-3</v>
+      </c>
+      <c r="T49" s="6">
+        <v>2.9146145137323061E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2003,8 +2458,18 @@
       <c r="O50" s="6">
         <v>3.6354363943475479E-2</v>
       </c>
-    </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R50" s="1">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S50" s="6">
+        <v>4.359918696240939E-3</v>
+      </c>
+      <c r="T50" s="6">
+        <v>2.9566440893823289E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2035,8 +2500,18 @@
       <c r="O51" s="6">
         <v>3.1746551808347588E-2</v>
       </c>
-    </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R51" s="1">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S51" s="6">
+        <v>4.378289801138119E-3</v>
+      </c>
+      <c r="T51" s="6">
+        <v>2.9945892998672011E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2067,8 +2542,18 @@
       <c r="O52" s="6">
         <v>3.3317772709260049E-2</v>
       </c>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R52" s="1">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S52" s="6">
+        <v>4.3804941163989239E-3</v>
+      </c>
+      <c r="T52" s="6">
+        <v>2.846213674644886E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2099,8 +2584,18 @@
       <c r="O53" s="6">
         <v>3.5742529622319587E-2</v>
       </c>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R53" s="1">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S53" s="6">
+        <v>4.3541708842635748E-3</v>
+      </c>
+      <c r="T53" s="6">
+        <v>2.8928877784643869E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2131,8 +2626,18 @@
       <c r="O54" s="6">
         <v>3.1921624442287702E-2</v>
       </c>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R54" s="1">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S54" s="6">
+        <v>4.1774023770928684E-3</v>
+      </c>
+      <c r="T54" s="6">
+        <v>3.0307708677298321E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2163,16 +2668,28 @@
       <c r="O55" s="6">
         <v>3.359791864684826E-2</v>
       </c>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R55" s="1">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S55" s="6">
+        <v>4.3811849785899528E-3</v>
+      </c>
+      <c r="T55" s="6">
+        <v>2.8186577575515001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+    </row>
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>20</v>
       </c>
@@ -2206,8 +2723,19 @@
         <f>AVERAGE(O6:O55)</f>
         <v>3.3039703875632175E-2</v>
       </c>
-    </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S57" s="6">
+        <f>AVERAGE(S6:S55)</f>
+        <v>4.260706060829015E-3</v>
+      </c>
+      <c r="T57" s="6">
+        <f>AVERAGE(T6:T55)</f>
+        <v>3.0397256840323766E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>21</v>
       </c>
@@ -2240,6 +2768,17 @@
       <c r="O58" s="6">
         <f>_xlfn.STDEV.S(O6:O55)</f>
         <v>2.189953442958352E-3</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S58" s="6">
+        <f>_xlfn.STDEV.S(S6:S55)</f>
+        <v>1.052240391066197E-4</v>
+      </c>
+      <c r="T58" s="6">
+        <f>_xlfn.STDEV.S(T6:T55)</f>
+        <v>1.9824912385534121E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2252,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,6 +2835,9 @@
       <c r="F5" s="3">
         <v>8.8413027272881861E-2</v>
       </c>
+      <c r="G5" s="3">
+        <v>9.6457275571641687E-2</v>
+      </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -2310,6 +2852,9 @@
       <c r="F6" s="3">
         <v>0.13328645042113921</v>
       </c>
+      <c r="G6" s="3">
+        <v>6.6980775082294039E-2</v>
+      </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -2324,6 +2869,9 @@
       <c r="F7" s="3">
         <v>7.9719945271623127E-2</v>
       </c>
+      <c r="G7" s="3">
+        <v>7.6812450108945468E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -2338,6 +2886,9 @@
       <c r="F8" s="3">
         <v>6.058922124692831E-2</v>
       </c>
+      <c r="G8" s="3">
+        <v>5.2896466336936523E-2</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -2352,6 +2903,9 @@
       <c r="F9" s="3">
         <v>5.6071573053039482E-2</v>
       </c>
+      <c r="G9" s="3">
+        <v>5.6349375325624271E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
@@ -2366,6 +2920,9 @@
       <c r="F10" s="3">
         <v>6.6070805140619762E-2</v>
       </c>
+      <c r="G10" s="3">
+        <v>7.9310227231377275E-2</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
@@ -2380,6 +2937,9 @@
       <c r="F11" s="3">
         <v>5.5571882969546488E-2</v>
       </c>
+      <c r="G11" s="3">
+        <v>7.1161695221062804E-2</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
@@ -2394,6 +2954,9 @@
       <c r="F12" s="3">
         <v>5.3242116681780208E-2</v>
       </c>
+      <c r="G12" s="3">
+        <v>4.9674828953573419E-2</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -2408,6 +2971,9 @@
       <c r="F13" s="3">
         <v>5.3475660887844681E-2</v>
       </c>
+      <c r="G13" s="3">
+        <v>4.6681826445339067E-2</v>
+      </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
@@ -2422,6 +2988,9 @@
       <c r="F14" s="3">
         <v>5.7848632447795943E-2</v>
       </c>
+      <c r="G14" s="3">
+        <v>5.9342486445714701E-2</v>
+      </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -2436,6 +3005,9 @@
       <c r="F15" s="3">
         <v>6.580257898426678E-2</v>
       </c>
+      <c r="G15" s="3">
+        <v>6.8842313663575128E-2</v>
+      </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
@@ -2450,8 +3022,11 @@
       <c r="F16" s="3">
         <v>6.0617071528018117E-2</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="3">
+        <v>8.6142539473756732E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2464,8 +3039,11 @@
       <c r="F17" s="3">
         <v>6.6874939593002225E-2</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="3">
+        <v>7.8110057307243894E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2478,8 +3056,11 @@
       <c r="F18" s="3">
         <v>3.7055712634370012E-2</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="3">
+        <v>3.6290434474359402E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2491,6 +3072,9 @@
       </c>
       <c r="F19" s="3">
         <v>6.5360381867143935E-2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>7.4947248358555735E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-16 total and regional saldo (balanced)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-16.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-16.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="mse (unbalanced set)" sheetId="1" r:id="rId1"/>
-    <sheet name="feature sig (unbalanced)" sheetId="2" r:id="rId2"/>
+    <sheet name="mse (balanced)" sheetId="3" r:id="rId2"/>
+    <sheet name="feature sig (unbalanced)" sheetId="2" r:id="rId3"/>
+    <sheet name="feature sig (balanced)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="32">
   <si>
     <t>features</t>
   </si>
@@ -107,6 +109,15 @@
   </si>
   <si>
     <t>significance</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 balanced.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 reg balanced.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 interreg balanced.csv)</t>
   </si>
 </sst>
 </file>
@@ -4439,8 +4450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AB58"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6764,10 +6775,1545 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:O57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5.3104753930396384E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3.8897944393984793E-2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6.043787684519521E-3</v>
+      </c>
+      <c r="J5" s="6">
+        <v>3.7007341400752222E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5.5622397378784329E-3</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3.1319610249867333E-2</v>
+      </c>
+      <c r="H6" s="1">
+        <f>H5+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5.947492627263351E-3</v>
+      </c>
+      <c r="J6" s="6">
+        <v>4.8061860030810637E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <f>M5+1</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5.5040312249622532E-3</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3.6493251349113728E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7:H54" si="1">H6+1</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5.6992892791531613E-3</v>
+      </c>
+      <c r="J7" s="6">
+        <v>4.501925008229362E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" ref="M7:M54" si="2">M6+1</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="6">
+        <v>5.5029682401868969E-3</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.5954763334794609E-2</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="6">
+        <v>6.0055766298190358E-3</v>
+      </c>
+      <c r="J8" s="6">
+        <v>4.221216870832533E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5.3220946365418022E-3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3.8111619243023538E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5.8823807908006311E-3</v>
+      </c>
+      <c r="J9" s="6">
+        <v>3.941517660216709E-2</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5.3180604973185807E-3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3.9815161815843492E-2</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5.823581255648998E-3</v>
+      </c>
+      <c r="J10" s="6">
+        <v>4.2703851996928402E-2</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5.4359656804684534E-3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3.490022953396154E-2</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="6">
+        <v>6.3468753793053589E-3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>3.5633443308147009E-2</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5.4473897875101504E-3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3.4064188260968402E-2</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="6">
+        <v>5.9255154597505607E-3</v>
+      </c>
+      <c r="J12" s="6">
+        <v>4.1415509879070778E-2</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.5276423846603428E-3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3.222583223226979E-2</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="6">
+        <v>5.6089995951911801E-3</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5.0896461798337997E-2</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="6">
+        <v>5.4774768417931909E-3</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3.3932767840322377E-2</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I14" s="6">
+        <v>5.8748029855858917E-3</v>
+      </c>
+      <c r="J14" s="6">
+        <v>4.7096861836770539E-2</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5.2047951217608253E-3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3.6972639439668657E-2</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I15" s="6">
+        <v>5.9801247696391804E-3</v>
+      </c>
+      <c r="J15" s="6">
+        <v>4.0219897424881759E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5.3553646070992958E-3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4.1330203183902882E-2</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="6">
+        <v>6.0390425584220444E-3</v>
+      </c>
+      <c r="J16" s="6">
+        <v>4.3182522686848343E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5.2204725279314194E-3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3.8778141911327252E-2</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I17" s="6">
+        <v>5.9889814094561504E-3</v>
+      </c>
+      <c r="J17" s="6">
+        <v>4.8365918505980522E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5.3245632119155346E-3</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4.0060019771525533E-2</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" s="6">
+        <v>5.8297220113767796E-3</v>
+      </c>
+      <c r="J18" s="6">
+        <v>4.4427254332486538E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="6">
+        <v>5.391817354262524E-3</v>
+      </c>
+      <c r="E19" s="6">
+        <v>3.7613754280585117E-2</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="6">
+        <v>5.7252919055045919E-3</v>
+      </c>
+      <c r="J19" s="6">
+        <v>4.89082869293559E-2</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="6">
+        <v>5.418287990897528E-3</v>
+      </c>
+      <c r="E20" s="6">
+        <v>3.5561676188384378E-2</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I20" s="6">
+        <v>6.1515188569774594E-3</v>
+      </c>
+      <c r="J20" s="6">
+        <v>3.4439139551836973E-2</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="6">
+        <v>5.1797307611916631E-3</v>
+      </c>
+      <c r="E21" s="6">
+        <v>4.1109650018466913E-2</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I21" s="6">
+        <v>5.6499196231562469E-3</v>
+      </c>
+      <c r="J21" s="6">
+        <v>5.0702093985400709E-2</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="6">
+        <v>5.1901342995441802E-3</v>
+      </c>
+      <c r="E22" s="6">
+        <v>3.7588612780899797E-2</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I22" s="6">
+        <v>6.1651819275118777E-3</v>
+      </c>
+      <c r="J22" s="6">
+        <v>4.2934307318328688E-2</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="6">
+        <v>5.2137860257953743E-3</v>
+      </c>
+      <c r="E23" s="6">
+        <v>4.1806069729942559E-2</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="6">
+        <v>6.1761641698526151E-3</v>
+      </c>
+      <c r="J23" s="6">
+        <v>4.01390529221533E-2</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="6">
+        <v>5.3928607189084026E-3</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3.528304599752189E-2</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="6">
+        <v>5.8162571903887083E-3</v>
+      </c>
+      <c r="J24" s="6">
+        <v>4.2686523832670908E-2</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="6">
+        <v>5.1658120142522839E-3</v>
+      </c>
+      <c r="E25" s="6">
+        <v>3.8583909059995938E-2</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5.7762100912324074E-3</v>
+      </c>
+      <c r="J25" s="6">
+        <v>4.5629081017939492E-2</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="6">
+        <v>5.3246992740949009E-3</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3.6992196277272169E-2</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I26" s="6">
+        <v>5.9160996291428873E-3</v>
+      </c>
+      <c r="J26" s="6">
+        <v>4.2860169766575723E-2</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="6">
+        <v>5.2486499002356718E-3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>3.5558813450606637E-2</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I27" s="6">
+        <v>6.1097367945461408E-3</v>
+      </c>
+      <c r="J27" s="6">
+        <v>3.5434831195968311E-2</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="6">
+        <v>5.4397690072115314E-3</v>
+      </c>
+      <c r="E28" s="6">
+        <v>3.4416553421128447E-2</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="6">
+        <v>6.1404226569137391E-3</v>
+      </c>
+      <c r="J28" s="6">
+        <v>3.7544348313272108E-2</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="6">
+        <v>5.4551084429111307E-3</v>
+      </c>
+      <c r="E29" s="6">
+        <v>3.6819103419234347E-2</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="6">
+        <v>6.0945296995915986E-3</v>
+      </c>
+      <c r="J29" s="6">
+        <v>3.6946678029657093E-2</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5.3473784083671238E-3</v>
+      </c>
+      <c r="E30" s="6">
+        <v>3.5317626729660379E-2</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I30" s="6">
+        <v>6.2513971780547009E-3</v>
+      </c>
+      <c r="J30" s="6">
+        <v>3.9611676819338013E-2</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="6">
+        <v>5.3156099794341031E-3</v>
+      </c>
+      <c r="E31" s="6">
+        <v>3.9843645578116503E-2</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="6">
+        <v>6.265315504502462E-3</v>
+      </c>
+      <c r="J31" s="6">
+        <v>3.8922445725583399E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5.1516020054665724E-3</v>
+      </c>
+      <c r="E32" s="6">
+        <v>3.7287493754049932E-2</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="6">
+        <v>6.2013142600634416E-3</v>
+      </c>
+      <c r="J32" s="6">
+        <v>4.4655024970186218E-2</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="6">
+        <v>5.2834275782727806E-3</v>
+      </c>
+      <c r="E33" s="6">
+        <v>3.6357354084474859E-2</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I33" s="6">
+        <v>5.7770858256022137E-3</v>
+      </c>
+      <c r="J33" s="6">
+        <v>4.272650224076327E-2</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="6">
+        <v>5.3058701929615979E-3</v>
+      </c>
+      <c r="E34" s="6">
+        <v>3.9491654790826412E-2</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I34" s="6">
+        <v>6.0841604325675511E-3</v>
+      </c>
+      <c r="J34" s="6">
+        <v>3.4254666302830597E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="6">
+        <v>5.0547268105089948E-3</v>
+      </c>
+      <c r="E35" s="6">
+        <v>4.3469373245170008E-2</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I35" s="6">
+        <v>6.0154146905993739E-3</v>
+      </c>
+      <c r="J35" s="6">
+        <v>3.8975763387265411E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="6">
+        <v>5.5650806155178823E-3</v>
+      </c>
+      <c r="E36" s="6">
+        <v>3.265094001107377E-2</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I36" s="6">
+        <v>5.8955224708575156E-3</v>
+      </c>
+      <c r="J36" s="6">
+        <v>4.6200042229924618E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="6">
+        <v>5.2388390258440078E-3</v>
+      </c>
+      <c r="E37" s="6">
+        <v>4.1731411866384641E-2</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="6">
+        <v>6.1276854182755131E-3</v>
+      </c>
+      <c r="J37" s="6">
+        <v>4.0706192794684418E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="6">
+        <v>5.2201483665199081E-3</v>
+      </c>
+      <c r="E38" s="6">
+        <v>3.7173214875095242E-2</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I38" s="6">
+        <v>6.127713562985684E-3</v>
+      </c>
+      <c r="J38" s="6">
+        <v>4.277507222685787E-2</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="6">
+        <v>5.5625205245708907E-3</v>
+      </c>
+      <c r="E39" s="6">
+        <v>3.2947155126045458E-2</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I39" s="6">
+        <v>5.7353127519684192E-3</v>
+      </c>
+      <c r="J39" s="6">
+        <v>4.1876028316187718E-2</v>
+      </c>
+      <c r="M39" s="1">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="6">
+        <v>5.3750531616386888E-3</v>
+      </c>
+      <c r="E40" s="6">
+        <v>4.13686079869846E-2</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I40" s="6">
+        <v>5.9557094193406698E-3</v>
+      </c>
+      <c r="J40" s="6">
+        <v>4.2249428918906998E-2</v>
+      </c>
+      <c r="M40" s="1">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="6">
+        <v>5.4470162721218501E-3</v>
+      </c>
+      <c r="E41" s="6">
+        <v>3.5901820831505657E-2</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I41" s="6">
+        <v>5.9556726149971604E-3</v>
+      </c>
+      <c r="J41" s="6">
+        <v>4.284307980888958E-2</v>
+      </c>
+      <c r="M41" s="1">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="6">
+        <v>5.5404466673291174E-3</v>
+      </c>
+      <c r="E42" s="6">
+        <v>3.090790890315364E-2</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I42" s="6">
+        <v>6.0758000552851533E-3</v>
+      </c>
+      <c r="J42" s="6">
+        <v>3.9162764326791458E-2</v>
+      </c>
+      <c r="M42" s="1">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="6">
+        <v>5.2438548744605084E-3</v>
+      </c>
+      <c r="E43" s="6">
+        <v>3.7990289271361867E-2</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I43" s="6">
+        <v>6.2309640923177666E-3</v>
+      </c>
+      <c r="J43" s="6">
+        <v>3.5614968585787742E-2</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="6">
+        <v>5.2254335410128966E-3</v>
+      </c>
+      <c r="E44" s="6">
+        <v>3.9659450411240159E-2</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I44" s="6">
+        <v>6.0065613187965773E-3</v>
+      </c>
+      <c r="J44" s="6">
+        <v>4.5966616768647682E-2</v>
+      </c>
+      <c r="M44" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="6">
+        <v>5.3053064518649674E-3</v>
+      </c>
+      <c r="E45" s="6">
+        <v>3.7274253971258442E-2</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="6">
+        <v>5.8604223953860309E-3</v>
+      </c>
+      <c r="J45" s="6">
+        <v>4.6455993366782293E-2</v>
+      </c>
+      <c r="M45" s="1">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="6">
+        <v>5.4891022262495608E-3</v>
+      </c>
+      <c r="E46" s="6">
+        <v>3.5634279373630777E-2</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I46" s="6">
+        <v>5.9565251174097094E-3</v>
+      </c>
+      <c r="J46" s="6">
+        <v>4.2606651780645877E-2</v>
+      </c>
+      <c r="M46" s="1">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C47" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="6">
+        <v>5.1056114547720667E-3</v>
+      </c>
+      <c r="E47" s="6">
+        <v>4.0395215622445163E-2</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I47" s="6">
+        <v>6.0718039782729277E-3</v>
+      </c>
+      <c r="J47" s="6">
+        <v>4.0373358234340607E-2</v>
+      </c>
+      <c r="M47" s="1">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="6">
+        <v>5.3012796456485102E-3</v>
+      </c>
+      <c r="E48" s="6">
+        <v>4.1055443509966497E-2</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I48" s="6">
+        <v>5.7923558590936338E-3</v>
+      </c>
+      <c r="J48" s="6">
+        <v>4.6711643423790743E-2</v>
+      </c>
+      <c r="M48" s="1">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="6">
+        <v>5.4720572190527341E-3</v>
+      </c>
+      <c r="E49" s="6">
+        <v>3.5415774238671788E-2</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I49" s="6">
+        <v>5.6168701945636286E-3</v>
+      </c>
+      <c r="J49" s="6">
+        <v>4.646555917015148E-2</v>
+      </c>
+      <c r="M49" s="1">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="6">
+        <v>5.2003187379554621E-3</v>
+      </c>
+      <c r="E50" s="6">
+        <v>3.7306434156995603E-2</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I50" s="6">
+        <v>5.6703129137548724E-3</v>
+      </c>
+      <c r="J50" s="6">
+        <v>4.5763583407194719E-2</v>
+      </c>
+      <c r="M50" s="1">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="6">
+        <v>5.2780810098806211E-3</v>
+      </c>
+      <c r="E51" s="6">
+        <v>3.9611667148375322E-2</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I51" s="6">
+        <v>5.8053922838071266E-3</v>
+      </c>
+      <c r="J51" s="6">
+        <v>4.6109005289492397E-2</v>
+      </c>
+      <c r="M51" s="1">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C52" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="6">
+        <v>5.5240145786112386E-3</v>
+      </c>
+      <c r="E52" s="6">
+        <v>3.1003509275187479E-2</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I52" s="6">
+        <v>5.8860458583245602E-3</v>
+      </c>
+      <c r="J52" s="6">
+        <v>4.1614338151178203E-2</v>
+      </c>
+      <c r="M52" s="1">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C53" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="6">
+        <v>5.1842033621296484E-3</v>
+      </c>
+      <c r="E53" s="6">
+        <v>3.6279494945906827E-2</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I53" s="6">
+        <v>5.9363417307535804E-3</v>
+      </c>
+      <c r="J53" s="6">
+        <v>3.9316385042013881E-2</v>
+      </c>
+      <c r="M53" s="1">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="6">
+        <v>5.1851771057237579E-3</v>
+      </c>
+      <c r="E54" s="6">
+        <v>3.8705367218879953E-2</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I54" s="6">
+        <v>6.2104373001206836E-3</v>
+      </c>
+      <c r="J54" s="6">
+        <v>4.1593730392167613E-2</v>
+      </c>
+      <c r="M54" s="1">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="6">
+        <f>AVERAGE(D5:D54)</f>
+        <v>5.3371271099657515E-3</v>
+      </c>
+      <c r="E56" s="6">
+        <f>AVERAGE(E5:E54)</f>
+        <v>3.7179382882221466E-2</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="6">
+        <f>AVERAGE(I5:I54)</f>
+        <v>5.9645928441690223E-3</v>
+      </c>
+      <c r="J56" s="6">
+        <f>AVERAGE(J5:J54)</f>
+        <v>4.2348651062747239E-2</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N56" s="6" t="e">
+        <f>AVERAGE(N5:N54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O56" s="6" t="e">
+        <f>AVERAGE(O5:O54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="6">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>1.3359025881010792E-4</v>
+      </c>
+      <c r="E57" s="6">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>2.9956006221870859E-3</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" s="6">
+        <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>1.8327215961586396E-4</v>
+      </c>
+      <c r="J57" s="6">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>4.1341298114801143E-3</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N57" s="6" t="e">
+        <f>_xlfn.STDEV.S(N5:N54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O57" s="6" t="e">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8041,4 +9587,236 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="7" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.880551163431764E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7.009837009815309E-2</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.0030121346806085E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.9346488238824067E-2</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.5198941028063002E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>6.8118220287461922E-2</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.8414927129624107E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.946362106638056E-2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6.1299686262342633E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6.395968675583473E-2</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8.7230214363094513E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7.600362760489443E-2</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.7817873706544842E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.1174849673092647E-2</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6.1434128827379482E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6.561314360654423E-2</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4.9118378090989658E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>6.0512384715106303E-2</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>6.5700560337304412E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7.6465718251584172E-2</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6.6902441843902136E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>6.1989727587624249E-2</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.669863272606682E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6.8882016258155584E-2</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>6.3401510547693496E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7.8203265854175599E-2</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>8.0165000874023645E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7.7253463572019621E-2</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>6.7782071281847434E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>6.2915416430148807E-2</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test-16 interreg. and internat saldo (balanced)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-16.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-16.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="mse (unbalanced set)" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="33">
   <si>
     <t>features</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24 interreg balanced.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 internat balanced.csv)</t>
   </si>
 </sst>
 </file>
@@ -6775,10 +6778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:O57"/>
+  <dimension ref="C3:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6789,9 +6792,11 @@
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6804,8 +6809,12 @@
         <v>31</v>
       </c>
       <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="5"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>18</v>
@@ -6827,8 +6836,15 @@
       <c r="O4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -6850,10 +6866,23 @@
       <c r="M5" s="1">
         <v>1</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N5" s="6">
+        <v>5.7305753897095206E-3</v>
+      </c>
+      <c r="O5" s="6">
+        <v>3.9960866387641833E-2</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="6">
+        <v>4.3662138808685819E-3</v>
+      </c>
+      <c r="T5" s="6">
+        <v>2.9985965477660081E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <f>C5+1</f>
         <v>2</v>
@@ -6878,10 +6907,24 @@
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="6">
+        <v>5.7447053667020109E-3</v>
+      </c>
+      <c r="O6" s="6">
+        <v>4.4013758837696502E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <f>R5+1</f>
+        <v>2</v>
+      </c>
+      <c r="S6" s="6">
+        <v>4.2960293946591316E-3</v>
+      </c>
+      <c r="T6" s="6">
+        <v>2.951424448553092E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -6906,10 +6949,24 @@
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="6">
+        <v>5.4590669561095607E-3</v>
+      </c>
+      <c r="O7" s="6">
+        <v>4.4144919593152712E-2</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" ref="R7:R54" si="3">R6+1</f>
+        <v>3</v>
+      </c>
+      <c r="S7" s="6">
+        <v>4.4274891780576907E-3</v>
+      </c>
+      <c r="T7" s="6">
+        <v>3.1658710303389591E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6934,10 +6991,24 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="6">
+        <v>5.5978129889899496E-3</v>
+      </c>
+      <c r="O8" s="6">
+        <v>4.0578830065683483E-2</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S8" s="6">
+        <v>4.2901890009543068E-3</v>
+      </c>
+      <c r="T8" s="6">
+        <v>3.1860866940451482E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6962,10 +7033,24 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="6">
+        <v>5.9006715495877231E-3</v>
+      </c>
+      <c r="O9" s="6">
+        <v>4.2292093948271228E-2</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="6">
+        <v>4.4113437762262472E-3</v>
+      </c>
+      <c r="T9" s="6">
+        <v>3.2009615547450819E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6990,10 +7075,24 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="6">
+        <v>5.5870086086319574E-3</v>
+      </c>
+      <c r="O10" s="6">
+        <v>4.2232775282372202E-2</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="6">
+        <v>4.3503367735446812E-3</v>
+      </c>
+      <c r="T10" s="6">
+        <v>3.2185489104264609E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7018,10 +7117,24 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N11" s="6">
+        <v>6.2350044118680177E-3</v>
+      </c>
+      <c r="O11" s="6">
+        <v>3.5463631205937887E-2</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S11" s="6">
+        <v>4.2275585365144398E-3</v>
+      </c>
+      <c r="T11" s="6">
+        <v>3.0316886111955349E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7046,10 +7159,24 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="6">
+        <v>5.821014603195303E-3</v>
+      </c>
+      <c r="O12" s="6">
+        <v>3.5594572517819563E-2</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="6">
+        <v>4.3100000359584901E-3</v>
+      </c>
+      <c r="T12" s="6">
+        <v>3.2475420820654063E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7074,10 +7201,24 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="6">
+        <v>5.7923149716504734E-3</v>
+      </c>
+      <c r="O13" s="6">
+        <v>3.7878637537360357E-2</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S13" s="6">
+        <v>4.2369706026830654E-3</v>
+      </c>
+      <c r="T13" s="6">
+        <v>3.0847881066197388E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7102,10 +7243,24 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="6">
+        <v>5.7482262722568433E-3</v>
+      </c>
+      <c r="O14" s="6">
+        <v>4.5697259524202408E-2</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S14" s="6">
+        <v>4.2757958751389862E-3</v>
+      </c>
+      <c r="T14" s="6">
+        <v>3.3976815764640102E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7130,10 +7285,24 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="6">
+        <v>5.7433791530156287E-3</v>
+      </c>
+      <c r="O15" s="6">
+        <v>4.0295685421102782E-2</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S15" s="6">
+        <v>4.3640940320787257E-3</v>
+      </c>
+      <c r="T15" s="6">
+        <v>2.959291827072803E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7158,10 +7327,24 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N16" s="6">
+        <v>5.597086656899457E-3</v>
+      </c>
+      <c r="O16" s="6">
+        <v>4.0651971757852852E-2</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S16" s="6">
+        <v>4.375715267146571E-3</v>
+      </c>
+      <c r="T16" s="6">
+        <v>3.0574381690624389E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7186,10 +7369,24 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="6">
+        <v>5.9285929975163576E-3</v>
+      </c>
+      <c r="O17" s="6">
+        <v>4.2309820448152659E-2</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S17" s="6">
+        <v>4.2041038166967474E-3</v>
+      </c>
+      <c r="T17" s="6">
+        <v>3.3384670759368268E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7214,10 +7411,24 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N18" s="6">
+        <v>5.8943100726015652E-3</v>
+      </c>
+      <c r="O18" s="6">
+        <v>3.5266142335318919E-2</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S18" s="6">
+        <v>4.4007446077116274E-3</v>
+      </c>
+      <c r="T18" s="6">
+        <v>3.063386368980392E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7242,10 +7453,24 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N19" s="6">
+        <v>5.5644189564140701E-3</v>
+      </c>
+      <c r="O19" s="6">
+        <v>4.6171643595542287E-2</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="6">
+        <v>4.4753524299497313E-3</v>
+      </c>
+      <c r="T19" s="6">
+        <v>3.0570468407808051E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7270,10 +7495,24 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N20" s="6">
+        <v>5.8890153111116729E-3</v>
+      </c>
+      <c r="O20" s="6">
+        <v>3.6635222972437258E-2</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S20" s="6">
+        <v>4.2676519187607011E-3</v>
+      </c>
+      <c r="T20" s="6">
+        <v>3.111174193716832E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7298,10 +7537,24 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="6">
+        <v>5.7755137718336824E-3</v>
+      </c>
+      <c r="O21" s="6">
+        <v>4.1727793885890679E-2</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S21" s="6">
+        <v>4.2608661169238789E-3</v>
+      </c>
+      <c r="T21" s="6">
+        <v>3.0284651729509591E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7326,10 +7579,24 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N22" s="6">
+        <v>5.7334649827576424E-3</v>
+      </c>
+      <c r="O22" s="6">
+        <v>4.324447699195428E-2</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S22" s="6">
+        <v>4.3767160279031634E-3</v>
+      </c>
+      <c r="T22" s="6">
+        <v>2.7637684029302102E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7354,10 +7621,24 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="6">
+        <v>5.6309212937625383E-3</v>
+      </c>
+      <c r="O23" s="6">
+        <v>4.7832210211685849E-2</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S23" s="6">
+        <v>4.4206478316873724E-3</v>
+      </c>
+      <c r="T23" s="6">
+        <v>2.7304587298147789E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7382,10 +7663,24 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="6">
+        <v>5.859658191694414E-3</v>
+      </c>
+      <c r="O24" s="6">
+        <v>4.2249477039927423E-2</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="6">
+        <v>4.4406672582620096E-3</v>
+      </c>
+      <c r="T24" s="6">
+        <v>3.1153019189014079E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7410,10 +7705,24 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N25" s="6">
+        <v>5.8465216677186576E-3</v>
+      </c>
+      <c r="O25" s="6">
+        <v>3.8443997180623857E-2</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="6">
+        <v>4.3497206228510898E-3</v>
+      </c>
+      <c r="T25" s="6">
+        <v>3.002094524710049E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7438,10 +7747,24 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N26" s="6">
+        <v>5.8241340549803388E-3</v>
+      </c>
+      <c r="O26" s="6">
+        <v>3.8900300506570541E-2</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S26" s="6">
+        <v>4.4543564931028481E-3</v>
+      </c>
+      <c r="T26" s="6">
+        <v>2.6358631698128781E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7466,10 +7789,24 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N27" s="6">
+        <v>5.7183875210084587E-3</v>
+      </c>
+      <c r="O27" s="6">
+        <v>4.1684666300918771E-2</v>
+      </c>
+      <c r="R27" s="1">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S27" s="6">
+        <v>4.4532715402303578E-3</v>
+      </c>
+      <c r="T27" s="6">
+        <v>3.1287350220378637E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7494,10 +7831,24 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N28" s="6">
+        <v>5.5328206230922097E-3</v>
+      </c>
+      <c r="O28" s="6">
+        <v>4.2039118446656629E-2</v>
+      </c>
+      <c r="R28" s="1">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="6">
+        <v>4.2971911806642116E-3</v>
+      </c>
+      <c r="T28" s="6">
+        <v>3.3146014495336648E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7522,10 +7873,24 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N29" s="6">
+        <v>5.7706914469083988E-3</v>
+      </c>
+      <c r="O29" s="6">
+        <v>4.5898485663434192E-2</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S29" s="6">
+        <v>4.2980976367610838E-3</v>
+      </c>
+      <c r="T29" s="6">
+        <v>3.2981749577565903E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -7550,10 +7915,24 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="6">
+        <v>5.9839424420553558E-3</v>
+      </c>
+      <c r="O30" s="6">
+        <v>3.82249731827582E-2</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S30" s="6">
+        <v>4.3512039102044566E-3</v>
+      </c>
+      <c r="T30" s="6">
+        <v>3.2200984801440333E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7578,10 +7957,24 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N31" s="6">
+        <v>5.7613807905654698E-3</v>
+      </c>
+      <c r="O31" s="6">
+        <v>4.1642472284809391E-2</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S31" s="6">
+        <v>4.4739409122262616E-3</v>
+      </c>
+      <c r="T31" s="6">
+        <v>2.739147779391219E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7606,10 +7999,24 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N32" s="6">
+        <v>5.9976584089296387E-3</v>
+      </c>
+      <c r="O32" s="6">
+        <v>3.435976658412019E-2</v>
+      </c>
+      <c r="R32" s="1">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S32" s="6">
+        <v>4.1792776943697131E-3</v>
+      </c>
+      <c r="T32" s="6">
+        <v>3.4341266320464567E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7634,10 +8041,24 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N33" s="6">
+        <v>5.9373562834768969E-3</v>
+      </c>
+      <c r="O33" s="6">
+        <v>3.8998214386947908E-2</v>
+      </c>
+      <c r="R33" s="1">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S33" s="6">
+        <v>4.2381245305853537E-3</v>
+      </c>
+      <c r="T33" s="6">
+        <v>3.2587852440111913E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7662,10 +8083,24 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N34" s="6">
+        <v>5.6618164870725022E-3</v>
+      </c>
+      <c r="O34" s="6">
+        <v>4.1968124945159738E-2</v>
+      </c>
+      <c r="R34" s="1">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S34" s="6">
+        <v>4.3114356345360346E-3</v>
+      </c>
+      <c r="T34" s="6">
+        <v>2.921405915234267E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7690,10 +8125,24 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="6">
+        <v>6.030553384939798E-3</v>
+      </c>
+      <c r="O35" s="6">
+        <v>3.025557430319404E-2</v>
+      </c>
+      <c r="R35" s="1">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S35" s="6">
+        <v>4.2062340055069626E-3</v>
+      </c>
+      <c r="T35" s="6">
+        <v>3.3823784512334067E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7718,10 +8167,24 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N36" s="6">
+        <v>5.974007041991288E-3</v>
+      </c>
+      <c r="O36" s="6">
+        <v>3.7668168847028567E-2</v>
+      </c>
+      <c r="R36" s="1">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S36" s="6">
+        <v>4.3552182852365064E-3</v>
+      </c>
+      <c r="T36" s="6">
+        <v>3.3483911123743479E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7746,10 +8209,24 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N37" s="6">
+        <v>5.549567445647636E-3</v>
+      </c>
+      <c r="O37" s="6">
+        <v>4.5740471762418043E-2</v>
+      </c>
+      <c r="R37" s="1">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S37" s="6">
+        <v>4.3533158793945953E-3</v>
+      </c>
+      <c r="T37" s="6">
+        <v>3.305702189590673E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7774,10 +8251,24 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N38" s="6">
+        <v>5.8254936715371117E-3</v>
+      </c>
+      <c r="O38" s="6">
+        <v>4.0616128604942708E-2</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S38" s="6">
+        <v>4.3987872365806027E-3</v>
+      </c>
+      <c r="T38" s="6">
+        <v>3.2976675060629138E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7802,10 +8293,24 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N39" s="6">
+        <v>5.67689081570826E-3</v>
+      </c>
+      <c r="O39" s="6">
+        <v>4.1783554139155833E-2</v>
+      </c>
+      <c r="R39" s="1">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S39" s="6">
+        <v>4.4116768569902676E-3</v>
+      </c>
+      <c r="T39" s="6">
+        <v>2.8086788772320841E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7830,10 +8335,24 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N40" s="6">
+        <v>5.4750243031827231E-3</v>
+      </c>
+      <c r="O40" s="6">
+        <v>4.6267962768873308E-2</v>
+      </c>
+      <c r="R40" s="1">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S40" s="6">
+        <v>4.3156568646947648E-3</v>
+      </c>
+      <c r="T40" s="6">
+        <v>2.9788187743657851E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7858,10 +8377,24 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N41" s="6">
+        <v>5.5641132981604034E-3</v>
+      </c>
+      <c r="O41" s="6">
+        <v>4.5486159743377753E-2</v>
+      </c>
+      <c r="R41" s="1">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S41" s="6">
+        <v>4.4760395294815838E-3</v>
+      </c>
+      <c r="T41" s="6">
+        <v>2.7464191759439569E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7886,10 +8419,24 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N42" s="6">
+        <v>5.8162006601476133E-3</v>
+      </c>
+      <c r="O42" s="6">
+        <v>3.5368105010515648E-2</v>
+      </c>
+      <c r="R42" s="1">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S42" s="6">
+        <v>4.3435753808785879E-3</v>
+      </c>
+      <c r="T42" s="6">
+        <v>2.7855653615923289E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7914,10 +8461,24 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N43" s="6">
+        <v>5.6671906406814297E-3</v>
+      </c>
+      <c r="O43" s="6">
+        <v>3.9925894776390747E-2</v>
+      </c>
+      <c r="R43" s="1">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S43" s="6">
+        <v>4.2051086184841649E-3</v>
+      </c>
+      <c r="T43" s="6">
+        <v>3.6304862960628258E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -7942,10 +8503,24 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N44" s="6">
+        <v>5.763424988369412E-3</v>
+      </c>
+      <c r="O44" s="6">
+        <v>4.4004641606101437E-2</v>
+      </c>
+      <c r="R44" s="1">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S44" s="6">
+        <v>4.1693140288612228E-3</v>
+      </c>
+      <c r="T44" s="6">
+        <v>3.471425046089404E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -7970,10 +8545,24 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N45" s="6">
+        <v>5.6989258432382636E-3</v>
+      </c>
+      <c r="O45" s="6">
+        <v>3.8110985349416468E-2</v>
+      </c>
+      <c r="R45" s="1">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S45" s="6">
+        <v>4.3313888075914306E-3</v>
+      </c>
+      <c r="T45" s="6">
+        <v>3.2008676469576607E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -7998,10 +8587,24 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N46" s="6">
+        <v>5.51175149377794E-3</v>
+      </c>
+      <c r="O46" s="6">
+        <v>4.5052057952169128E-2</v>
+      </c>
+      <c r="R46" s="1">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S46" s="6">
+        <v>4.2336551973933528E-3</v>
+      </c>
+      <c r="T46" s="6">
+        <v>3.1269355348684788E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -8026,10 +8629,24 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N47" s="6">
+        <v>5.6234869012480758E-3</v>
+      </c>
+      <c r="O47" s="6">
+        <v>4.1909240795953789E-2</v>
+      </c>
+      <c r="R47" s="1">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S47" s="6">
+        <v>4.2935053786866831E-3</v>
+      </c>
+      <c r="T47" s="6">
+        <v>2.9995156424125081E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -8054,10 +8671,24 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N48" s="6">
+        <v>6.0319115184099019E-3</v>
+      </c>
+      <c r="O48" s="6">
+        <v>3.3549913525840407E-2</v>
+      </c>
+      <c r="R48" s="1">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S48" s="6">
+        <v>4.5298441879509646E-3</v>
+      </c>
+      <c r="T48" s="6">
+        <v>2.9112908377452829E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -8082,10 +8713,24 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-    </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N49" s="6">
+        <v>5.9164907794115474E-3</v>
+      </c>
+      <c r="O49" s="6">
+        <v>3.2155787338743837E-2</v>
+      </c>
+      <c r="R49" s="1">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S49" s="6">
+        <v>4.2348972118724298E-3</v>
+      </c>
+      <c r="T49" s="6">
+        <v>3.3526425668171288E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -8110,10 +8755,24 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-    </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N50" s="6">
+        <v>5.85249884249493E-3</v>
+      </c>
+      <c r="O50" s="6">
+        <v>3.7557052799183567E-2</v>
+      </c>
+      <c r="R50" s="1">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S50" s="6">
+        <v>4.3616248258358309E-3</v>
+      </c>
+      <c r="T50" s="6">
+        <v>2.9636017090601631E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -8138,10 +8797,24 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-    </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N51" s="6">
+        <v>5.427263061098378E-3</v>
+      </c>
+      <c r="O51" s="6">
+        <v>4.8106270548171487E-2</v>
+      </c>
+      <c r="R51" s="1">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S51" s="6">
+        <v>4.3242255365788526E-3</v>
+      </c>
+      <c r="T51" s="6">
+        <v>3.0610959123951099E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -8166,10 +8839,24 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N52" s="6">
+        <v>6.0687889741324504E-3</v>
+      </c>
+      <c r="O52" s="6">
+        <v>4.0262084150918531E-2</v>
+      </c>
+      <c r="R52" s="1">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S52" s="6">
+        <v>4.2100792435240328E-3</v>
+      </c>
+      <c r="T52" s="6">
+        <v>3.1746329279091663E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -8194,10 +8881,24 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N53" s="6">
+        <v>5.593546086319302E-3</v>
+      </c>
+      <c r="O53" s="6">
+        <v>4.4771896217957748E-2</v>
+      </c>
+      <c r="R53" s="1">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S53" s="6">
+        <v>3.9938461389336013E-3</v>
+      </c>
+      <c r="T53" s="6">
+        <v>3.7565983818053782E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -8222,18 +8923,34 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N54" s="6">
+        <v>5.7414574717971041E-3</v>
+      </c>
+      <c r="O54" s="6">
+        <v>4.3074088043551763E-2</v>
+      </c>
+      <c r="R54" s="1">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S54" s="6">
+        <v>4.325491633084563E-3</v>
+      </c>
+      <c r="T54" s="6">
+        <v>3.4029027863765472E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+    </row>
+    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>20</v>
       </c>
@@ -8259,16 +8976,27 @@
       <c r="M56" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N56" s="6" t="e">
+      <c r="N56" s="6">
         <f>AVERAGE(N5:N54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O56" s="6" t="e">
+        <v>5.7615211890881968E-3</v>
+      </c>
+      <c r="O56" s="6">
         <f>AVERAGE(O5:O54)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+        <v>4.0761358946518146E-2</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S56" s="6">
+        <f>AVERAGE(S5:S54)</f>
+        <v>4.3251718272963712E-3</v>
+      </c>
+      <c r="T56" s="6">
+        <f>AVERAGE(T5:T54)</f>
+        <v>3.1273327634788038E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>21</v>
       </c>
@@ -8294,13 +9022,24 @@
       <c r="M57" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N57" s="6" t="e">
+      <c r="N57" s="6">
         <f>_xlfn.STDEV.S(N5:N54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O57" s="6" t="e">
+        <v>1.7481947264513244E-4</v>
+      </c>
+      <c r="O57" s="6">
         <f>_xlfn.STDEV.S(O5:O54)</f>
-        <v>#DIV/0!</v>
+        <v>4.0932925358896956E-3</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S57" s="6">
+        <f>_xlfn.STDEV.S(S5:S54)</f>
+        <v>9.9317799287817991E-5</v>
+      </c>
+      <c r="T57" s="6">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>2.365660764892532E-3</v>
       </c>
     </row>
   </sheetData>
@@ -8313,7 +9052,7 @@
   <dimension ref="C4:V95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:N9"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9593,15 +10332,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
@@ -9631,8 +10371,12 @@
       <c r="E5" s="3">
         <v>7.009837009815309E-2</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3">
+        <v>7.6358303495708033E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>7.5310073050020909E-2</v>
+      </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -9644,8 +10388,12 @@
       <c r="E6" s="3">
         <v>5.9346488238824067E-2</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3">
+        <v>8.2996736548339098E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>6.8349343660667167E-2</v>
+      </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -9657,8 +10405,12 @@
       <c r="E7" s="3">
         <v>6.8118220287461922E-2</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3">
+        <v>7.8410784282839166E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8.3776915890514947E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -9670,8 +10422,12 @@
       <c r="E8" s="3">
         <v>4.946362106638056E-2</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3">
+        <v>5.0546691880879652E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5.2697404827940733E-2</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -9683,8 +10439,12 @@
       <c r="E9" s="3">
         <v>6.395968675583473E-2</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3">
+        <v>6.3354941029826681E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6.6126765735793056E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
@@ -9696,8 +10456,12 @@
       <c r="E10" s="3">
         <v>7.600362760489443E-2</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3">
+        <v>6.932226853197837E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8.5405569473412268E-2</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
@@ -9709,8 +10473,12 @@
       <c r="E11" s="3">
         <v>6.1174849673092647E-2</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="3">
+        <v>5.4128810024916332E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>7.596673881253603E-2</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
@@ -9722,8 +10490,12 @@
       <c r="E12" s="3">
         <v>6.561314360654423E-2</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="3">
+        <v>5.5319417047725861E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5.5104918809272728E-2</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -9735,8 +10507,12 @@
       <c r="E13" s="3">
         <v>6.0512384715106303E-2</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="F13" s="3">
+        <v>8.9968939378246737E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5.1873252896754707E-2</v>
+      </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
@@ -9748,8 +10524,12 @@
       <c r="E14" s="3">
         <v>7.6465718251584172E-2</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3">
+        <v>5.5831400688950622E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5.8672785197884207E-2</v>
+      </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -9761,8 +10541,12 @@
       <c r="E15" s="3">
         <v>6.1989727587624249E-2</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="F15" s="3">
+        <v>8.040294682165823E-2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>7.0847902836447818E-2</v>
+      </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
@@ -9774,8 +10558,12 @@
       <c r="E16" s="3">
         <v>6.8882016258155584E-2</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="3">
+        <v>6.8995896296658379E-2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>8.106354082024278E-2</v>
+      </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
@@ -9787,8 +10575,12 @@
       <c r="E17" s="3">
         <v>7.8203265854175599E-2</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="3">
+        <v>7.0034349413396008E-2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>7.5200229031547383E-2</v>
+      </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
@@ -9800,8 +10592,12 @@
       <c r="E18" s="3">
         <v>7.7253463572019621E-2</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="3">
+        <v>4.2327607921780988E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3.8305152016196838E-2</v>
+      </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
@@ -9813,8 +10609,12 @@
       <c r="E19" s="3">
         <v>6.2915416430148807E-2</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="3">
+        <v>6.2000906637095857E-2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6.1299406940768401E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test-16 significance of features (balanced)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-16.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-16.xlsx
@@ -12,6 +12,15 @@
     <sheet name="feature sig (unbalanced)" sheetId="2" r:id="rId3"/>
     <sheet name="feature sig (balanced)" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'feature sig (balanced)'!$S$5:$S$19</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'feature sig (balanced)'!$T$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'feature sig (balanced)'!$T$5:$T$19</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'feature sig (balanced)'!$U$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'feature sig (balanced)'!$U$5:$U$19</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'feature sig (balanced)'!$V$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'feature sig (balanced)'!$V$5:$V$19</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -22,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="35">
   <si>
     <t>features</t>
   </si>
@@ -122,6 +131,12 @@
   <si>
     <t>Random Forest-100 (superdataset-24 internat balanced.csv)</t>
   </si>
+  <si>
+    <t>Несбалансированные выборки</t>
+  </si>
+  <si>
+    <t>Сбалансированные выборки</t>
+  </si>
 </sst>
 </file>
 
@@ -160,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +194,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,6 +248,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1898,6 +1931,638 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'feature sig (balanced)'!$T$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>regional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'feature sig (balanced)'!$S$5:$S$19</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'feature sig (balanced)'!$T$5:$T$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7.009837009815309E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9346488238824067E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8118220287461922E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.946362106638056E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.395968675583473E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.600362760489443E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1174849673092647E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.561314360654423E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0512384715106303E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6465718251584172E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.1989727587624249E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8882016258155584E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.8203265854175599E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.7253463572019621E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.2915416430148807E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-395B-42BE-BE52-B29F64A213CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'feature sig (balanced)'!$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>interregional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'feature sig (balanced)'!$S$5:$S$19</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'feature sig (balanced)'!$U$5:$U$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7.6358303495708033E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2996736548339098E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8410784282839166E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0546691880879652E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3354941029826681E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.932226853197837E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4128810024916332E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5319417047725861E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9968939378246737E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5831400688950622E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.040294682165823E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8995896296658379E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0034349413396008E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2327607921780988E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.2000906637095857E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-395B-42BE-BE52-B29F64A213CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'feature sig (balanced)'!$V$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>international</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'feature sig (balanced)'!$S$5:$S$19</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'feature sig (balanced)'!$V$5:$V$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7.5310073050020909E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8349343660667167E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3776915890514947E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2697404827940733E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6126765735793056E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5405569473412268E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.596673881253603E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5104918809272728E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1873252896754707E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8672785197884207E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.0847902836447818E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.106354082024278E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.5200229031547383E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8305152016196838E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.1299406940768401E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-395B-42BE-BE52-B29F64A213CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="634066576"/>
+        <c:axId val="634073232"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="634066576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634073232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="634073232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634066576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2058,6 +2723,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
   <cs:axisTitle>
@@ -4055,6 +4760,511 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4180,6 +5390,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>96371</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>201706</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9049,10 +10294,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:V95"/>
+  <dimension ref="C3:V95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9072,6 +10317,11 @@
     <col min="19" max="19" width="16" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="L3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -10330,21 +11580,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:G19"/>
+  <dimension ref="C3:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="6" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="L3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -10360,8 +11623,32 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
@@ -10377,8 +11664,32 @@
       <c r="G5" s="3">
         <v>7.5310073050020909E-2</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>7.009837009815309E-2</v>
+      </c>
+      <c r="U5" s="3">
+        <v>7.6358303495708033E-2</v>
+      </c>
+      <c r="V5" s="3">
+        <v>7.5310073050020909E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -10394,8 +11705,33 @@
       <c r="G6" s="3">
         <v>6.8349343660667167E-2</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K6" s="8">
+        <f>K5+1</f>
+        <v>2</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="3">
+        <v>5.9346488238824067E-2</v>
+      </c>
+      <c r="U6" s="3">
+        <v>8.2996736548339098E-2</v>
+      </c>
+      <c r="V6" s="3">
+        <v>6.8349343660667167E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
@@ -10411,8 +11747,33 @@
       <c r="G7" s="3">
         <v>8.3776915890514947E-2</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K7" s="8">
+        <f t="shared" ref="K7:K19" si="0">K6+1</f>
+        <v>3</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T7" s="3">
+        <v>6.8118220287461922E-2</v>
+      </c>
+      <c r="U7" s="3">
+        <v>7.8410784282839166E-2</v>
+      </c>
+      <c r="V7" s="3">
+        <v>8.3776915890514947E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -10428,8 +11789,33 @@
       <c r="G8" s="3">
         <v>5.2697404827940733E-2</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K8" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="3">
+        <v>4.946362106638056E-2</v>
+      </c>
+      <c r="U8" s="3">
+        <v>5.0546691880879652E-2</v>
+      </c>
+      <c r="V8" s="3">
+        <v>5.2697404827940733E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
@@ -10445,8 +11831,33 @@
       <c r="G9" s="3">
         <v>6.6126765735793056E-2</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K9" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T9" s="3">
+        <v>6.395968675583473E-2</v>
+      </c>
+      <c r="U9" s="3">
+        <v>6.3354941029826681E-2</v>
+      </c>
+      <c r="V9" s="3">
+        <v>6.6126765735793056E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
@@ -10462,8 +11873,33 @@
       <c r="G10" s="3">
         <v>8.5405569473412268E-2</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K10" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" s="3">
+        <v>7.600362760489443E-2</v>
+      </c>
+      <c r="U10" s="3">
+        <v>6.932226853197837E-2</v>
+      </c>
+      <c r="V10" s="3">
+        <v>8.5405569473412268E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -10479,8 +11915,33 @@
       <c r="G11" s="3">
         <v>7.596673881253603E-2</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K11" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T11" s="3">
+        <v>6.1174849673092647E-2</v>
+      </c>
+      <c r="U11" s="3">
+        <v>5.4128810024916332E-2</v>
+      </c>
+      <c r="V11" s="3">
+        <v>7.596673881253603E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
@@ -10496,8 +11957,33 @@
       <c r="G12" s="3">
         <v>5.5104918809272728E-2</v>
       </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K12" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="3">
+        <v>6.561314360654423E-2</v>
+      </c>
+      <c r="U12" s="3">
+        <v>5.5319417047725861E-2</v>
+      </c>
+      <c r="V12" s="3">
+        <v>5.5104918809272728E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -10513,8 +11999,33 @@
       <c r="G13" s="3">
         <v>5.1873252896754707E-2</v>
       </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K13" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T13" s="3">
+        <v>6.0512384715106303E-2</v>
+      </c>
+      <c r="U13" s="3">
+        <v>8.9968939378246737E-2</v>
+      </c>
+      <c r="V13" s="3">
+        <v>5.1873252896754707E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
@@ -10530,8 +12041,33 @@
       <c r="G14" s="3">
         <v>5.8672785197884207E-2</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K14" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T14" s="3">
+        <v>7.6465718251584172E-2</v>
+      </c>
+      <c r="U14" s="3">
+        <v>5.5831400688950622E-2</v>
+      </c>
+      <c r="V14" s="3">
+        <v>5.8672785197884207E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
@@ -10547,8 +12083,33 @@
       <c r="G15" s="3">
         <v>7.0847902836447818E-2</v>
       </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K15" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T15" s="3">
+        <v>6.1989727587624249E-2</v>
+      </c>
+      <c r="U15" s="3">
+        <v>8.040294682165823E-2</v>
+      </c>
+      <c r="V15" s="3">
+        <v>7.0847902836447818E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
@@ -10564,8 +12125,33 @@
       <c r="G16" s="3">
         <v>8.106354082024278E-2</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K16" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="3">
+        <v>6.8882016258155584E-2</v>
+      </c>
+      <c r="U16" s="3">
+        <v>6.8995896296658379E-2</v>
+      </c>
+      <c r="V16" s="3">
+        <v>8.106354082024278E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
@@ -10581,8 +12167,33 @@
       <c r="G17" s="3">
         <v>7.5200229031547383E-2</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K17" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T17" s="3">
+        <v>7.8203265854175599E-2</v>
+      </c>
+      <c r="U17" s="3">
+        <v>7.0034349413396008E-2</v>
+      </c>
+      <c r="V17" s="3">
+        <v>7.5200229031547383E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
@@ -10598,8 +12209,33 @@
       <c r="G18" s="3">
         <v>3.8305152016196838E-2</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="K18" s="8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T18" s="3">
+        <v>7.7253463572019621E-2</v>
+      </c>
+      <c r="U18" s="3">
+        <v>4.2327607921780988E-2</v>
+      </c>
+      <c r="V18" s="3">
+        <v>3.8305152016196838E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
@@ -10615,8 +12251,373 @@
       <c r="G19" s="3">
         <v>6.1299406940768401E-2</v>
       </c>
+      <c r="K19" s="8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T19" s="3">
+        <v>6.2915416430148807E-2</v>
+      </c>
+      <c r="U19" s="3">
+        <v>6.2000906637095857E-2</v>
+      </c>
+      <c r="V19" s="3">
+        <v>6.1299406940768401E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="3">
+        <v>7.8203265854175599E-2</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="3">
+        <v>8.9968939378246737E-2</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="3">
+        <v>8.5405569473412268E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="3">
+        <v>7.7253463572019621E-2</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3">
+        <v>8.2996736548339098E-2</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>8.3776915890514947E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3">
+        <v>7.6465718251584172E-2</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="3">
+        <v>8.040294682165823E-2</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="3">
+        <v>8.106354082024278E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3">
+        <v>7.600362760489443E-2</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="3">
+        <v>7.8410784282839166E-2</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="3">
+        <v>7.596673881253603E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>7.009837009815309E-2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>7.6358303495708033E-2</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>7.5310073050020909E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3">
+        <v>6.8882016258155584E-2</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="3">
+        <v>7.0034349413396008E-2</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="3">
+        <v>7.5200229031547383E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3">
+        <v>6.8118220287461922E-2</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="3">
+        <v>6.932226853197837E-2</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="3">
+        <v>7.0847902836447818E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="3">
+        <v>6.561314360654423E-2</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="3">
+        <v>6.8995896296658379E-2</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="3">
+        <v>6.8349343660667167E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3">
+        <v>6.395968675583473E-2</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="3">
+        <v>6.3354941029826681E-2</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="3">
+        <v>6.6126765735793056E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="3">
+        <v>6.2915416430148807E-2</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="3">
+        <v>6.2000906637095857E-2</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="3">
+        <v>6.1299406940768401E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="3">
+        <v>6.1989727587624249E-2</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="3">
+        <v>5.5831400688950622E-2</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="3">
+        <v>5.8672785197884207E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6.1174849673092647E-2</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="3">
+        <v>5.5319417047725861E-2</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="3">
+        <v>5.5104918809272728E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
+        <v>6.0512384715106303E-2</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="3">
+        <v>5.4128810024916332E-2</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="3">
+        <v>5.2697404827940733E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5.9346488238824067E-2</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3">
+        <v>5.0546691880879652E-2</v>
+      </c>
+      <c r="H40" s="3"/>
+      <c r="I40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40" s="3">
+        <v>5.1873252896754707E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="3">
+        <v>4.946362106638056E-2</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="3">
+        <v>4.2327607921780988E-2</v>
+      </c>
+      <c r="H41" s="3"/>
+      <c r="I41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="3">
+        <v>3.8305152016196838E-2</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="I27:J41">
+    <sortCondition descending="1" ref="J27:J41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>